<commit_message>
manager search and sort
</commit_message>
<xml_diff>
--- a/fuying/src/assets/others/data_template(前端视角数据文档).xlsx
+++ b/fuying/src/assets/others/data_template(前端视角数据文档).xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Desktop\fuying\fuying\fuying\src\assets\others\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C5BC9F2-25AB-4604-B7CD-9EBDF7C97AE4}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A74AFD04-91A7-483A-ABDC-F4629AD76FD0}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="579" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="766" uniqueCount="428">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="771" uniqueCount="433">
   <si>
     <t>应用页面</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -1676,13 +1676,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>post
-(要求接受一个id
-确认是否为adminId，
-否则返回空值)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>*更换了url头
 头部为https://phenomics.fudan.edu.cn/firmiana/health/api/
 api为get_all_report</t>
@@ -1692,6 +1685,31 @@
     <t>*更换了url头
 头部为https://phenomics.fudan.edu.cn/firmiana/health/api/
 api为get_pdf</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>传递参数及说明</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>id(string)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>filter(dict)
+通用域anyfield</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>sort/property</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>get</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>sort/direction(DESC/ASC)</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1823,7 +1841,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="53">
+  <cellXfs count="55">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1954,6 +1972,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1961,19 +1982,22 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1997,13 +2021,13 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>5</xdr:col>
+      <xdr:col>6</xdr:col>
       <xdr:colOff>314325</xdr:colOff>
       <xdr:row>120</xdr:row>
       <xdr:rowOff>66675</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>12</xdr:col>
+      <xdr:col>13</xdr:col>
       <xdr:colOff>3055747</xdr:colOff>
       <xdr:row>151</xdr:row>
       <xdr:rowOff>36945</xdr:rowOff>
@@ -2047,8 +2071,8 @@
       <xdr:rowOff>47625</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>313130</xdr:colOff>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>1122755</xdr:colOff>
       <xdr:row>135</xdr:row>
       <xdr:rowOff>17895</xdr:rowOff>
     </xdr:to>
@@ -2091,8 +2115,8 @@
       <xdr:rowOff>95250</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>313130</xdr:colOff>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>1122755</xdr:colOff>
       <xdr:row>177</xdr:row>
       <xdr:rowOff>65522</xdr:rowOff>
     </xdr:to>
@@ -2129,13 +2153,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>5</xdr:col>
+      <xdr:col>6</xdr:col>
       <xdr:colOff>1009650</xdr:colOff>
       <xdr:row>164</xdr:row>
       <xdr:rowOff>104775</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>13</xdr:col>
+      <xdr:col>14</xdr:col>
       <xdr:colOff>178614</xdr:colOff>
       <xdr:row>195</xdr:row>
       <xdr:rowOff>75045</xdr:rowOff>
@@ -2179,8 +2203,8 @@
       <xdr:rowOff>9525</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>313130</xdr:colOff>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>1122755</xdr:colOff>
       <xdr:row>219</xdr:row>
       <xdr:rowOff>160771</xdr:rowOff>
     </xdr:to>
@@ -2217,13 +2241,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>5</xdr:col>
+      <xdr:col>6</xdr:col>
       <xdr:colOff>495300</xdr:colOff>
       <xdr:row>214</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>12</xdr:col>
+      <xdr:col>13</xdr:col>
       <xdr:colOff>3236722</xdr:colOff>
       <xdr:row>244</xdr:row>
       <xdr:rowOff>151246</xdr:rowOff>
@@ -2267,8 +2291,8 @@
       <xdr:rowOff>171450</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>313130</xdr:colOff>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>1122755</xdr:colOff>
       <xdr:row>270</xdr:row>
       <xdr:rowOff>141721</xdr:rowOff>
     </xdr:to>
@@ -2305,13 +2329,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>5</xdr:col>
+      <xdr:col>6</xdr:col>
       <xdr:colOff>904875</xdr:colOff>
       <xdr:row>265</xdr:row>
       <xdr:rowOff>9525</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>13</xdr:col>
+      <xdr:col>14</xdr:col>
       <xdr:colOff>73839</xdr:colOff>
       <xdr:row>295</xdr:row>
       <xdr:rowOff>160771</xdr:rowOff>
@@ -2613,24 +2637,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:M107"/>
+  <dimension ref="A1:N107"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A78" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B101" sqref="A101:XFD101"/>
+    <sheetView tabSelected="1" topLeftCell="A79" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E98" sqref="E98"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
     <col min="1" max="1" width="9" style="8"/>
-    <col min="2" max="4" width="20.625" style="8" customWidth="1"/>
-    <col min="5" max="5" width="23.25" style="27" customWidth="1"/>
-    <col min="6" max="9" width="15.625" style="9" customWidth="1"/>
-    <col min="10" max="11" width="9" style="9"/>
-    <col min="12" max="12" width="28.625" style="20" customWidth="1"/>
-    <col min="13" max="13" width="47" style="9" customWidth="1"/>
+    <col min="2" max="5" width="20.625" style="8" customWidth="1"/>
+    <col min="6" max="6" width="23.25" style="27" customWidth="1"/>
+    <col min="7" max="10" width="15.625" style="9" customWidth="1"/>
+    <col min="11" max="12" width="9" style="9"/>
+    <col min="13" max="13" width="28.625" style="20" customWidth="1"/>
+    <col min="14" max="14" width="47" style="9" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" s="8" customFormat="1">
+    <row r="1" spans="1:14" s="8" customFormat="1">
       <c r="A1" s="8" t="s">
         <v>42</v>
       </c>
@@ -2643,232 +2667,241 @@
       <c r="D1" s="8" t="s">
         <v>255</v>
       </c>
-      <c r="E1" s="27" t="s">
+      <c r="E1" s="8" t="s">
+        <v>427</v>
+      </c>
+      <c r="F1" s="27" t="s">
         <v>67</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="L1" s="19" t="s">
+      <c r="M1" s="19" t="s">
         <v>125</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="2" spans="1:13" ht="15" customHeight="1">
-      <c r="A2" s="45" t="s">
+    <row r="2" spans="1:14" ht="15" customHeight="1">
+      <c r="A2" s="49" t="s">
         <v>44</v>
       </c>
-      <c r="B2" s="45" t="s">
+      <c r="B2" s="49" t="s">
         <v>64</v>
       </c>
-      <c r="C2" s="45" t="s">
+      <c r="C2" s="49" t="s">
         <v>45</v>
       </c>
-      <c r="D2" s="48" t="s">
+      <c r="D2" s="50" t="s">
         <v>56</v>
       </c>
-      <c r="E2" s="27" t="s">
+      <c r="E2" s="46"/>
+      <c r="F2" s="27" t="s">
         <v>12</v>
       </c>
-      <c r="F2" s="6" t="s">
+      <c r="G2" s="6" t="s">
         <v>46</v>
       </c>
-      <c r="G2" s="6" t="s">
+      <c r="H2" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="H2" s="6" t="s">
+      <c r="I2" s="6" t="s">
         <v>48</v>
       </c>
-      <c r="I2" s="6" t="b">
+      <c r="J2" s="6" t="b">
         <v>1</v>
       </c>
-      <c r="J2" s="6" t="s">
-        <v>40</v>
-      </c>
       <c r="K2" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="L2" s="51" t="s">
+      <c r="L2" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="M2" s="52" t="s">
         <v>126</v>
       </c>
-      <c r="M2" s="6"/>
-    </row>
-    <row r="3" spans="1:13">
-      <c r="A3" s="45"/>
-      <c r="B3" s="45"/>
-      <c r="C3" s="45"/>
-      <c r="D3" s="45"/>
-      <c r="E3" s="27" t="s">
+      <c r="N2" s="6"/>
+    </row>
+    <row r="3" spans="1:14">
+      <c r="A3" s="49"/>
+      <c r="B3" s="49"/>
+      <c r="C3" s="49"/>
+      <c r="D3" s="49"/>
+      <c r="E3" s="45"/>
+      <c r="F3" s="27" t="s">
         <v>12</v>
       </c>
-      <c r="F3" s="6" t="s">
+      <c r="G3" s="6" t="s">
         <v>49</v>
       </c>
-      <c r="G3" s="6" t="s">
+      <c r="H3" s="6" t="s">
         <v>50</v>
       </c>
-      <c r="H3" s="6" t="s">
+      <c r="I3" s="6" t="s">
         <v>48</v>
       </c>
-      <c r="I3" s="6" t="b">
+      <c r="J3" s="6" t="b">
         <v>1</v>
       </c>
-      <c r="J3" s="6" t="s">
-        <v>40</v>
-      </c>
       <c r="K3" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="L3" s="51"/>
-      <c r="M3" s="6"/>
-    </row>
-    <row r="4" spans="1:13">
-      <c r="A4" s="45"/>
-      <c r="B4" s="45"/>
-      <c r="C4" s="45"/>
-      <c r="D4" s="45"/>
-      <c r="E4" s="27" t="s">
+      <c r="L3" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="M3" s="52"/>
+      <c r="N3" s="6"/>
+    </row>
+    <row r="4" spans="1:14">
+      <c r="A4" s="49"/>
+      <c r="B4" s="49"/>
+      <c r="C4" s="49"/>
+      <c r="D4" s="49"/>
+      <c r="E4" s="45"/>
+      <c r="F4" s="27" t="s">
         <v>12</v>
       </c>
-      <c r="F4" s="6" t="s">
+      <c r="G4" s="6" t="s">
         <v>51</v>
       </c>
-      <c r="G4" s="6" t="s">
+      <c r="H4" s="6" t="s">
         <v>52</v>
       </c>
-      <c r="H4" s="6" t="s">
+      <c r="I4" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="I4" s="6" t="s">
+      <c r="J4" s="6" t="s">
         <v>53</v>
       </c>
-      <c r="J4" s="6" t="s">
-        <v>40</v>
-      </c>
       <c r="K4" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="L4" s="51"/>
-      <c r="M4" s="6"/>
-    </row>
-    <row r="5" spans="1:13">
-      <c r="A5" s="45"/>
-      <c r="B5" s="45"/>
-      <c r="C5" s="45"/>
-      <c r="D5" s="45"/>
-      <c r="E5" s="27" t="s">
+      <c r="L4" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="M4" s="52"/>
+      <c r="N4" s="6"/>
+    </row>
+    <row r="5" spans="1:14">
+      <c r="A5" s="49"/>
+      <c r="B5" s="49"/>
+      <c r="C5" s="49"/>
+      <c r="D5" s="49"/>
+      <c r="E5" s="45"/>
+      <c r="F5" s="27" t="s">
         <v>12</v>
       </c>
-      <c r="F5" s="6" t="s">
+      <c r="G5" s="6" t="s">
         <v>54</v>
       </c>
-      <c r="G5" s="6" t="s">
+      <c r="H5" s="6" t="s">
         <v>55</v>
       </c>
-      <c r="H5" s="6" t="s">
+      <c r="I5" s="6" t="s">
         <v>48</v>
       </c>
-      <c r="I5" s="6" t="b">
+      <c r="J5" s="6" t="b">
         <v>0</v>
-      </c>
-      <c r="J5" s="6" t="s">
-        <v>97</v>
       </c>
       <c r="K5" s="6" t="s">
         <v>97</v>
       </c>
-      <c r="L5" s="51"/>
-      <c r="M5" s="6" t="s">
+      <c r="L5" s="6" t="s">
+        <v>97</v>
+      </c>
+      <c r="M5" s="52"/>
+      <c r="N5" s="6" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="6" spans="1:13" ht="35.1" customHeight="1">
-      <c r="A6" s="45"/>
-      <c r="B6" s="45" t="s">
+    <row r="6" spans="1:14" ht="35.1" customHeight="1">
+      <c r="A6" s="49"/>
+      <c r="B6" s="49" t="s">
         <v>65</v>
       </c>
-      <c r="C6" s="45" t="s">
+      <c r="C6" s="49" t="s">
         <v>57</v>
       </c>
-      <c r="D6" s="48" t="s">
+      <c r="D6" s="50" t="s">
         <v>62</v>
       </c>
-      <c r="E6" s="27" t="s">
+      <c r="E6" s="46"/>
+      <c r="F6" s="27" t="s">
         <v>12</v>
       </c>
-      <c r="F6" s="6" t="s">
+      <c r="G6" s="6" t="s">
         <v>46</v>
       </c>
-      <c r="G6" s="6" t="s">
+      <c r="H6" s="6" t="s">
         <v>58</v>
       </c>
-      <c r="H6" s="6" t="s">
+      <c r="I6" s="6" t="s">
         <v>48</v>
       </c>
-      <c r="I6" s="6" t="b">
+      <c r="J6" s="6" t="b">
         <v>1</v>
       </c>
-      <c r="J6" s="6" t="s">
-        <v>40</v>
-      </c>
       <c r="K6" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="L6" s="51" t="s">
+      <c r="L6" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="M6" s="52" t="s">
         <v>128</v>
       </c>
-      <c r="M6" s="6"/>
-    </row>
-    <row r="7" spans="1:13" ht="35.1" customHeight="1">
-      <c r="A7" s="45"/>
-      <c r="B7" s="45"/>
-      <c r="C7" s="45"/>
-      <c r="D7" s="45"/>
-      <c r="E7" s="27" t="s">
+      <c r="N6" s="6"/>
+    </row>
+    <row r="7" spans="1:14" ht="35.1" customHeight="1">
+      <c r="A7" s="49"/>
+      <c r="B7" s="49"/>
+      <c r="C7" s="49"/>
+      <c r="D7" s="49"/>
+      <c r="E7" s="45"/>
+      <c r="F7" s="27" t="s">
         <v>12</v>
       </c>
-      <c r="F7" s="6" t="s">
+      <c r="G7" s="6" t="s">
         <v>51</v>
       </c>
-      <c r="G7" s="6" t="s">
+      <c r="H7" s="6" t="s">
         <v>59</v>
       </c>
-      <c r="H7" s="6" t="s">
+      <c r="I7" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="I7" s="6" t="s">
+      <c r="J7" s="6" t="s">
         <v>60</v>
-      </c>
-      <c r="J7" s="6" t="s">
-        <v>97</v>
       </c>
       <c r="K7" s="6" t="s">
         <v>97</v>
       </c>
-      <c r="L7" s="51"/>
-      <c r="M7" s="6" t="s">
+      <c r="L7" s="6" t="s">
+        <v>97</v>
+      </c>
+      <c r="M7" s="52"/>
+      <c r="N7" s="6" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="8" spans="1:13" s="3" customFormat="1" ht="28.5">
-      <c r="A8" s="45"/>
+    <row r="8" spans="1:14" s="3" customFormat="1" ht="28.5">
+      <c r="A8" s="49"/>
       <c r="B8" s="4" t="s">
         <v>66</v>
       </c>
@@ -2878,933 +2911,965 @@
       <c r="D8" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="E8" s="2" t="s">
+      <c r="E8" s="4"/>
+      <c r="F8" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="F8" s="5" t="s">
+      <c r="G8" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="G8" s="5"/>
       <c r="H8" s="5"/>
       <c r="I8" s="5"/>
-      <c r="J8" s="5" t="s">
-        <v>40</v>
-      </c>
+      <c r="J8" s="5"/>
       <c r="K8" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="L8" s="21" t="s">
+      <c r="L8" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="M8" s="21" t="s">
         <v>127</v>
       </c>
-      <c r="M8" s="5"/>
-    </row>
-    <row r="9" spans="1:13" ht="15" customHeight="1">
-      <c r="A9" s="45" t="s">
+      <c r="N8" s="5"/>
+    </row>
+    <row r="9" spans="1:14" ht="15" customHeight="1">
+      <c r="A9" s="49" t="s">
         <v>43</v>
       </c>
-      <c r="B9" s="48" t="s">
+      <c r="B9" s="50" t="s">
         <v>69</v>
       </c>
-      <c r="C9" s="48" t="s">
+      <c r="C9" s="50" t="s">
         <v>15</v>
       </c>
-      <c r="D9" s="48" t="s">
+      <c r="D9" s="50" t="s">
         <v>117</v>
       </c>
-      <c r="E9" s="45" t="s">
+      <c r="E9" s="46"/>
+      <c r="F9" s="49" t="s">
         <v>136</v>
       </c>
-      <c r="F9" s="6" t="s">
+      <c r="G9" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="G9" s="6" t="s">
+      <c r="H9" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="H9" s="6" t="s">
+      <c r="I9" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="I9" s="6" t="s">
+      <c r="J9" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="J9" s="6" t="s">
-        <v>40</v>
-      </c>
       <c r="K9" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="L9" s="6" t="s">
         <v>97</v>
       </c>
-      <c r="L9" s="51" t="s">
+      <c r="M9" s="52" t="s">
         <v>130</v>
       </c>
-      <c r="M9" s="6"/>
-    </row>
-    <row r="10" spans="1:13">
-      <c r="A10" s="45"/>
-      <c r="B10" s="45"/>
-      <c r="C10" s="45"/>
-      <c r="D10" s="45"/>
+      <c r="N9" s="6"/>
+    </row>
+    <row r="10" spans="1:14">
+      <c r="A10" s="49"/>
+      <c r="B10" s="49"/>
+      <c r="C10" s="49"/>
+      <c r="D10" s="49"/>
       <c r="E10" s="45"/>
-      <c r="F10" s="6" t="s">
+      <c r="F10" s="49"/>
+      <c r="G10" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="G10" s="6" t="s">
+      <c r="H10" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="H10" s="6" t="s">
+      <c r="I10" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="I10" s="6" t="s">
+      <c r="J10" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="J10" s="6" t="s">
-        <v>40</v>
-      </c>
       <c r="K10" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="L10" s="6" t="s">
         <v>97</v>
       </c>
-      <c r="L10" s="51"/>
-      <c r="M10" s="6"/>
-    </row>
-    <row r="11" spans="1:13">
-      <c r="A11" s="45"/>
-      <c r="B11" s="45"/>
-      <c r="C11" s="45"/>
-      <c r="D11" s="45"/>
+      <c r="M10" s="52"/>
+      <c r="N10" s="6"/>
+    </row>
+    <row r="11" spans="1:14">
+      <c r="A11" s="49"/>
+      <c r="B11" s="49"/>
+      <c r="C11" s="49"/>
+      <c r="D11" s="49"/>
       <c r="E11" s="45"/>
-      <c r="F11" s="11" t="s">
+      <c r="F11" s="49"/>
+      <c r="G11" s="11" t="s">
         <v>93</v>
       </c>
-      <c r="G11" s="11" t="s">
+      <c r="H11" s="11" t="s">
         <v>94</v>
       </c>
-      <c r="H11" s="11" t="s">
+      <c r="I11" s="11" t="s">
         <v>95</v>
       </c>
-      <c r="I11" s="11" t="s">
+      <c r="J11" s="11" t="s">
         <v>96</v>
-      </c>
-      <c r="J11" s="11" t="s">
-        <v>97</v>
       </c>
       <c r="K11" s="11" t="s">
         <v>97</v>
       </c>
-      <c r="L11" s="51"/>
-      <c r="M11" s="11"/>
-    </row>
-    <row r="12" spans="1:13">
-      <c r="A12" s="45"/>
-      <c r="B12" s="45"/>
-      <c r="C12" s="45"/>
-      <c r="D12" s="45"/>
+      <c r="L11" s="11" t="s">
+        <v>97</v>
+      </c>
+      <c r="M11" s="52"/>
+      <c r="N11" s="11"/>
+    </row>
+    <row r="12" spans="1:14">
+      <c r="A12" s="49"/>
+      <c r="B12" s="49"/>
+      <c r="C12" s="49"/>
+      <c r="D12" s="49"/>
       <c r="E12" s="45"/>
-      <c r="F12" s="6" t="s">
+      <c r="F12" s="49"/>
+      <c r="G12" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="G12" s="6" t="s">
+      <c r="H12" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="H12" s="6" t="s">
+      <c r="I12" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="I12" s="6" t="s">
+      <c r="J12" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="J12" s="6" t="s">
-        <v>40</v>
-      </c>
       <c r="K12" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="L12" s="6" t="s">
         <v>97</v>
       </c>
-      <c r="L12" s="51"/>
-      <c r="M12" s="6" t="s">
+      <c r="M12" s="52"/>
+      <c r="N12" s="6" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="13" spans="1:13" ht="15" customHeight="1">
-      <c r="A13" s="45"/>
-      <c r="B13" s="48" t="s">
+    <row r="13" spans="1:14" ht="15" customHeight="1">
+      <c r="A13" s="49"/>
+      <c r="B13" s="50" t="s">
         <v>70</v>
       </c>
-      <c r="C13" s="48" t="s">
+      <c r="C13" s="50" t="s">
         <v>16</v>
       </c>
-      <c r="D13" s="48" t="s">
+      <c r="D13" s="50" t="s">
         <v>132</v>
       </c>
-      <c r="E13" s="27" t="s">
+      <c r="E13" s="46"/>
+      <c r="F13" s="27" t="s">
         <v>12</v>
       </c>
-      <c r="F13" s="6" t="s">
+      <c r="G13" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="G13" s="6" t="s">
+      <c r="H13" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="H13" s="6" t="s">
+      <c r="I13" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="I13" s="6" t="s">
+      <c r="J13" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="J13" s="6" t="s">
-        <v>40</v>
-      </c>
-      <c r="K13" s="14" t="s">
-        <v>40</v>
-      </c>
-      <c r="L13" s="51" t="s">
+      <c r="K13" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="L13" s="14" t="s">
+        <v>40</v>
+      </c>
+      <c r="M13" s="52" t="s">
         <v>129</v>
       </c>
-      <c r="M13" s="6"/>
-    </row>
-    <row r="14" spans="1:13">
-      <c r="A14" s="45"/>
-      <c r="B14" s="48"/>
-      <c r="C14" s="48"/>
-      <c r="D14" s="48"/>
-      <c r="E14" s="27" t="s">
+      <c r="N13" s="6"/>
+    </row>
+    <row r="14" spans="1:14">
+      <c r="A14" s="49"/>
+      <c r="B14" s="50"/>
+      <c r="C14" s="50"/>
+      <c r="D14" s="50"/>
+      <c r="E14" s="46"/>
+      <c r="F14" s="27" t="s">
         <v>12</v>
       </c>
-      <c r="F14" s="6" t="s">
+      <c r="G14" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="G14" s="6" t="s">
+      <c r="H14" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="H14" s="6" t="s">
+      <c r="I14" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="I14" s="6" t="s">
+      <c r="J14" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="J14" s="6" t="s">
-        <v>40</v>
-      </c>
-      <c r="K14" s="14" t="s">
-        <v>40</v>
-      </c>
-      <c r="L14" s="51"/>
-      <c r="M14" s="6"/>
-    </row>
-    <row r="15" spans="1:13">
-      <c r="A15" s="45"/>
-      <c r="B15" s="48"/>
-      <c r="C15" s="48"/>
-      <c r="D15" s="48"/>
-      <c r="E15" s="27" t="s">
+      <c r="K14" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="L14" s="14" t="s">
+        <v>40</v>
+      </c>
+      <c r="M14" s="52"/>
+      <c r="N14" s="6"/>
+    </row>
+    <row r="15" spans="1:14">
+      <c r="A15" s="49"/>
+      <c r="B15" s="50"/>
+      <c r="C15" s="50"/>
+      <c r="D15" s="50"/>
+      <c r="E15" s="46"/>
+      <c r="F15" s="27" t="s">
         <v>12</v>
       </c>
-      <c r="F15" s="14" t="s">
+      <c r="G15" s="14" t="s">
         <v>106</v>
       </c>
-      <c r="G15" s="14" t="s">
+      <c r="H15" s="14" t="s">
         <v>107</v>
       </c>
-      <c r="H15" s="14" t="s">
+      <c r="I15" s="14" t="s">
         <v>71</v>
       </c>
-      <c r="I15" s="14" t="s">
+      <c r="J15" s="14" t="s">
         <v>108</v>
       </c>
-      <c r="J15" s="14"/>
       <c r="K15" s="14"/>
-      <c r="L15" s="51"/>
-      <c r="M15" s="14"/>
-    </row>
-    <row r="16" spans="1:13">
-      <c r="A16" s="45"/>
-      <c r="B16" s="48"/>
-      <c r="C16" s="48"/>
-      <c r="D16" s="48"/>
-      <c r="E16" s="45" t="s">
+      <c r="L15" s="14"/>
+      <c r="M15" s="52"/>
+      <c r="N15" s="14"/>
+    </row>
+    <row r="16" spans="1:14">
+      <c r="A16" s="49"/>
+      <c r="B16" s="50"/>
+      <c r="C16" s="50"/>
+      <c r="D16" s="50"/>
+      <c r="E16" s="46"/>
+      <c r="F16" s="49" t="s">
         <v>137</v>
       </c>
-      <c r="F16" s="6" t="s">
+      <c r="G16" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="G16" s="6" t="s">
+      <c r="H16" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="H16" s="6" t="s">
+      <c r="I16" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="I16" s="6" t="s">
+      <c r="J16" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="J16" s="6" t="s">
-        <v>40</v>
-      </c>
       <c r="K16" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="L16" s="6" t="s">
         <v>109</v>
       </c>
-      <c r="L16" s="51"/>
-      <c r="M16" s="6"/>
-    </row>
-    <row r="17" spans="1:13">
-      <c r="A17" s="45"/>
-      <c r="B17" s="48"/>
-      <c r="C17" s="48"/>
-      <c r="D17" s="48"/>
-      <c r="E17" s="45"/>
-      <c r="F17" s="6" t="s">
+      <c r="M16" s="52"/>
+      <c r="N16" s="6"/>
+    </row>
+    <row r="17" spans="1:14">
+      <c r="A17" s="49"/>
+      <c r="B17" s="50"/>
+      <c r="C17" s="50"/>
+      <c r="D17" s="50"/>
+      <c r="E17" s="46"/>
+      <c r="F17" s="49"/>
+      <c r="G17" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="G17" s="6" t="s">
+      <c r="H17" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="H17" s="6" t="s">
+      <c r="I17" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="I17" s="6" t="s">
+      <c r="J17" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="J17" s="6" t="s">
-        <v>40</v>
-      </c>
-      <c r="K17" s="15" t="s">
+      <c r="K17" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="L17" s="15" t="s">
         <v>109</v>
       </c>
-      <c r="L17" s="51"/>
-      <c r="M17" s="6"/>
-    </row>
-    <row r="18" spans="1:13">
-      <c r="A18" s="45"/>
-      <c r="B18" s="48"/>
-      <c r="C18" s="48"/>
-      <c r="D18" s="48"/>
-      <c r="E18" s="45"/>
-      <c r="F18" s="6" t="s">
+      <c r="M17" s="52"/>
+      <c r="N17" s="6"/>
+    </row>
+    <row r="18" spans="1:14">
+      <c r="A18" s="49"/>
+      <c r="B18" s="50"/>
+      <c r="C18" s="50"/>
+      <c r="D18" s="50"/>
+      <c r="E18" s="46"/>
+      <c r="F18" s="49"/>
+      <c r="G18" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="G18" s="6" t="s">
+      <c r="H18" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="H18" s="6" t="s">
+      <c r="I18" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="I18" s="6" t="s">
+      <c r="J18" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="J18" s="6" t="s">
-        <v>40</v>
-      </c>
-      <c r="K18" s="15" t="s">
+      <c r="K18" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="L18" s="15" t="s">
         <v>109</v>
       </c>
-      <c r="L18" s="51"/>
-      <c r="M18" s="6"/>
-    </row>
-    <row r="19" spans="1:13">
-      <c r="A19" s="45"/>
-      <c r="B19" s="48"/>
-      <c r="C19" s="48"/>
-      <c r="D19" s="48"/>
-      <c r="E19" s="45"/>
-      <c r="F19" s="6" t="s">
+      <c r="M18" s="52"/>
+      <c r="N18" s="6"/>
+    </row>
+    <row r="19" spans="1:14">
+      <c r="A19" s="49"/>
+      <c r="B19" s="50"/>
+      <c r="C19" s="50"/>
+      <c r="D19" s="50"/>
+      <c r="E19" s="46"/>
+      <c r="F19" s="49"/>
+      <c r="G19" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="G19" s="6" t="s">
+      <c r="H19" s="6" t="s">
         <v>82</v>
       </c>
-      <c r="H19" s="6" t="s">
+      <c r="I19" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="I19" s="10">
+      <c r="J19" s="10">
         <v>100</v>
       </c>
-      <c r="J19" s="6" t="s">
-        <v>40</v>
-      </c>
-      <c r="K19" s="15" t="s">
+      <c r="K19" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="L19" s="15" t="s">
         <v>109</v>
       </c>
-      <c r="L19" s="51"/>
-      <c r="M19" s="6"/>
-    </row>
-    <row r="20" spans="1:13">
-      <c r="A20" s="45"/>
-      <c r="B20" s="48"/>
-      <c r="C20" s="48"/>
-      <c r="D20" s="48"/>
-      <c r="E20" s="45" t="s">
+      <c r="M19" s="52"/>
+      <c r="N19" s="6"/>
+    </row>
+    <row r="20" spans="1:14">
+      <c r="A20" s="49"/>
+      <c r="B20" s="50"/>
+      <c r="C20" s="50"/>
+      <c r="D20" s="50"/>
+      <c r="E20" s="46"/>
+      <c r="F20" s="49" t="s">
         <v>33</v>
       </c>
-      <c r="F20" s="6" t="s">
+      <c r="G20" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="G20" s="6" t="s">
+      <c r="H20" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="H20" s="6" t="s">
+      <c r="I20" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="I20" s="6" t="s">
+      <c r="J20" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="J20" s="6" t="s">
-        <v>40</v>
-      </c>
-      <c r="K20" s="15" t="s">
+      <c r="K20" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="L20" s="15" t="s">
         <v>109</v>
       </c>
-      <c r="L20" s="51"/>
-      <c r="M20" s="6"/>
-    </row>
-    <row r="21" spans="1:13">
-      <c r="A21" s="45"/>
-      <c r="B21" s="48"/>
-      <c r="C21" s="48"/>
-      <c r="D21" s="48"/>
-      <c r="E21" s="45"/>
-      <c r="F21" s="6" t="s">
+      <c r="M20" s="52"/>
+      <c r="N20" s="6"/>
+    </row>
+    <row r="21" spans="1:14">
+      <c r="A21" s="49"/>
+      <c r="B21" s="50"/>
+      <c r="C21" s="50"/>
+      <c r="D21" s="50"/>
+      <c r="E21" s="46"/>
+      <c r="F21" s="49"/>
+      <c r="G21" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="G21" s="6" t="s">
+      <c r="H21" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="H21" s="6" t="s">
+      <c r="I21" s="6" t="s">
         <v>71</v>
       </c>
-      <c r="I21" s="6" t="s">
+      <c r="J21" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="J21" s="6" t="s">
-        <v>40</v>
-      </c>
-      <c r="K21" s="15" t="s">
+      <c r="K21" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="L21" s="15" t="s">
         <v>109</v>
       </c>
-      <c r="L21" s="51"/>
-      <c r="M21" s="11" t="s">
+      <c r="M21" s="52"/>
+      <c r="N21" s="11" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="22" spans="1:13" ht="14.25" customHeight="1">
-      <c r="A22" s="45" t="s">
+    <row r="22" spans="1:14" ht="14.25" customHeight="1">
+      <c r="A22" s="49" t="s">
         <v>63</v>
       </c>
-      <c r="B22" s="45" t="s">
+      <c r="B22" s="49" t="s">
         <v>72</v>
       </c>
-      <c r="C22" s="48" t="s">
+      <c r="C22" s="50" t="s">
         <v>86</v>
       </c>
-      <c r="D22" s="48" t="s">
+      <c r="D22" s="50" t="s">
         <v>133</v>
       </c>
-      <c r="E22" s="45" t="s">
+      <c r="E22" s="46"/>
+      <c r="F22" s="49" t="s">
         <v>73</v>
       </c>
-      <c r="F22" s="6" t="s">
+      <c r="G22" s="6" t="s">
         <v>111</v>
       </c>
-      <c r="G22" s="6" t="s">
+      <c r="H22" s="6" t="s">
         <v>74</v>
       </c>
-      <c r="H22" s="6" t="s">
+      <c r="I22" s="6" t="s">
         <v>76</v>
       </c>
-      <c r="I22" s="6" t="s">
+      <c r="J22" s="6" t="s">
         <v>77</v>
       </c>
-      <c r="J22" s="11" t="s">
-        <v>40</v>
-      </c>
-      <c r="K22" s="18" t="s">
-        <v>40</v>
-      </c>
-      <c r="L22" s="51" t="s">
+      <c r="K22" s="11" t="s">
+        <v>40</v>
+      </c>
+      <c r="L22" s="18" t="s">
+        <v>40</v>
+      </c>
+      <c r="M22" s="52" t="s">
         <v>131</v>
       </c>
-      <c r="M22" s="6"/>
-    </row>
-    <row r="23" spans="1:13" ht="14.25" customHeight="1">
-      <c r="A23" s="45"/>
-      <c r="B23" s="45"/>
-      <c r="C23" s="48"/>
-      <c r="D23" s="48"/>
-      <c r="E23" s="45"/>
-      <c r="F23" s="7" t="s">
+      <c r="N22" s="6"/>
+    </row>
+    <row r="23" spans="1:14" ht="14.25" customHeight="1">
+      <c r="A23" s="49"/>
+      <c r="B23" s="49"/>
+      <c r="C23" s="50"/>
+      <c r="D23" s="50"/>
+      <c r="E23" s="46"/>
+      <c r="F23" s="49"/>
+      <c r="G23" s="7" t="s">
         <v>112</v>
       </c>
-      <c r="G23" s="7" t="s">
+      <c r="H23" s="7" t="s">
         <v>87</v>
       </c>
-      <c r="H23" s="7" t="s">
+      <c r="I23" s="7" t="s">
         <v>76</v>
       </c>
-      <c r="I23" s="7" t="s">
+      <c r="J23" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="J23" s="11" t="s">
-        <v>40</v>
-      </c>
-      <c r="K23" s="18" t="s">
-        <v>40</v>
-      </c>
-      <c r="L23" s="51"/>
-      <c r="M23" s="7"/>
-    </row>
-    <row r="24" spans="1:13" ht="14.25" customHeight="1">
-      <c r="A24" s="45"/>
-      <c r="B24" s="45"/>
-      <c r="C24" s="48"/>
-      <c r="D24" s="48"/>
-      <c r="E24" s="45"/>
-      <c r="F24" s="9" t="s">
+      <c r="K23" s="11" t="s">
+        <v>40</v>
+      </c>
+      <c r="L23" s="18" t="s">
+        <v>40</v>
+      </c>
+      <c r="M23" s="52"/>
+      <c r="N23" s="7"/>
+    </row>
+    <row r="24" spans="1:14" ht="14.25" customHeight="1">
+      <c r="A24" s="49"/>
+      <c r="B24" s="49"/>
+      <c r="C24" s="50"/>
+      <c r="D24" s="50"/>
+      <c r="E24" s="46"/>
+      <c r="F24" s="49"/>
+      <c r="G24" s="9" t="s">
         <v>113</v>
       </c>
-      <c r="G24" s="6" t="s">
+      <c r="H24" s="6" t="s">
         <v>75</v>
       </c>
-      <c r="H24" s="6" t="s">
+      <c r="I24" s="6" t="s">
         <v>76</v>
       </c>
-      <c r="I24" s="6" t="s">
+      <c r="J24" s="6" t="s">
         <v>78</v>
       </c>
-      <c r="J24" s="11" t="s">
-        <v>40</v>
-      </c>
-      <c r="K24" s="18" t="s">
-        <v>40</v>
-      </c>
-      <c r="L24" s="51"/>
-      <c r="M24" s="6"/>
-    </row>
-    <row r="25" spans="1:13" ht="14.25" customHeight="1">
-      <c r="A25" s="45"/>
-      <c r="B25" s="45"/>
-      <c r="C25" s="48"/>
-      <c r="D25" s="48"/>
-      <c r="E25" s="45"/>
-      <c r="F25" s="9" t="s">
+      <c r="K24" s="11" t="s">
+        <v>40</v>
+      </c>
+      <c r="L24" s="18" t="s">
+        <v>40</v>
+      </c>
+      <c r="M24" s="52"/>
+      <c r="N24" s="6"/>
+    </row>
+    <row r="25" spans="1:14" ht="14.25" customHeight="1">
+      <c r="A25" s="49"/>
+      <c r="B25" s="49"/>
+      <c r="C25" s="50"/>
+      <c r="D25" s="50"/>
+      <c r="E25" s="46"/>
+      <c r="F25" s="49"/>
+      <c r="G25" s="9" t="s">
         <v>114</v>
       </c>
-      <c r="G25" s="7" t="s">
+      <c r="H25" s="7" t="s">
         <v>88</v>
       </c>
-      <c r="H25" s="7" t="s">
+      <c r="I25" s="7" t="s">
         <v>76</v>
       </c>
-      <c r="I25" s="7" t="s">
+      <c r="J25" s="7" t="s">
         <v>89</v>
       </c>
-      <c r="J25" s="11" t="s">
-        <v>40</v>
-      </c>
-      <c r="K25" s="18" t="s">
-        <v>40</v>
-      </c>
-      <c r="L25" s="51"/>
-      <c r="M25" s="7"/>
-    </row>
-    <row r="26" spans="1:13" ht="14.25" customHeight="1">
-      <c r="A26" s="45"/>
-      <c r="B26" s="45"/>
-      <c r="C26" s="48"/>
-      <c r="D26" s="48"/>
-      <c r="E26" s="45"/>
-      <c r="F26" s="9" t="s">
+      <c r="K25" s="11" t="s">
+        <v>40</v>
+      </c>
+      <c r="L25" s="18" t="s">
+        <v>40</v>
+      </c>
+      <c r="M25" s="52"/>
+      <c r="N25" s="7"/>
+    </row>
+    <row r="26" spans="1:14" ht="14.25" customHeight="1">
+      <c r="A26" s="49"/>
+      <c r="B26" s="49"/>
+      <c r="C26" s="50"/>
+      <c r="D26" s="50"/>
+      <c r="E26" s="46"/>
+      <c r="F26" s="49"/>
+      <c r="G26" s="9" t="s">
         <v>115</v>
       </c>
-      <c r="G26" s="9" t="s">
+      <c r="H26" s="9" t="s">
         <v>79</v>
       </c>
-      <c r="H26" s="9" t="s">
+      <c r="I26" s="9" t="s">
         <v>76</v>
       </c>
-      <c r="I26" s="9" t="s">
+      <c r="J26" s="9" t="s">
         <v>80</v>
       </c>
-      <c r="J26" s="11" t="s">
-        <v>40</v>
-      </c>
-      <c r="K26" s="18" t="s">
-        <v>40</v>
-      </c>
-      <c r="L26" s="51"/>
-      <c r="M26" s="11" t="s">
+      <c r="K26" s="11" t="s">
+        <v>40</v>
+      </c>
+      <c r="L26" s="18" t="s">
+        <v>40</v>
+      </c>
+      <c r="M26" s="52"/>
+      <c r="N26" s="11" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="27" spans="1:13" ht="14.25" customHeight="1">
-      <c r="A27" s="45"/>
-      <c r="B27" s="45"/>
-      <c r="C27" s="48"/>
-      <c r="D27" s="48"/>
-      <c r="E27" s="45"/>
-      <c r="F27" s="9" t="s">
+    <row r="27" spans="1:14" ht="14.25" customHeight="1">
+      <c r="A27" s="49"/>
+      <c r="B27" s="49"/>
+      <c r="C27" s="50"/>
+      <c r="D27" s="50"/>
+      <c r="E27" s="46"/>
+      <c r="F27" s="49"/>
+      <c r="G27" s="9" t="s">
         <v>81</v>
       </c>
-      <c r="G27" s="9" t="s">
+      <c r="H27" s="9" t="s">
         <v>83</v>
       </c>
-      <c r="H27" s="9" t="s">
+      <c r="I27" s="9" t="s">
         <v>84</v>
       </c>
-      <c r="I27" s="10">
+      <c r="J27" s="10">
         <v>100</v>
       </c>
-      <c r="J27" s="11" t="s">
-        <v>40</v>
-      </c>
-      <c r="K27" s="18" t="s">
-        <v>40</v>
-      </c>
-      <c r="L27" s="51"/>
-    </row>
-    <row r="28" spans="1:13" ht="14.25" customHeight="1">
-      <c r="A28" s="45"/>
-      <c r="B28" s="45"/>
-      <c r="C28" s="48"/>
-      <c r="D28" s="48"/>
-      <c r="E28" s="45"/>
-      <c r="F28" s="9" t="s">
+      <c r="K27" s="11" t="s">
+        <v>40</v>
+      </c>
+      <c r="L27" s="18" t="s">
+        <v>40</v>
+      </c>
+      <c r="M27" s="52"/>
+    </row>
+    <row r="28" spans="1:14" ht="14.25" customHeight="1">
+      <c r="A28" s="49"/>
+      <c r="B28" s="49"/>
+      <c r="C28" s="50"/>
+      <c r="D28" s="50"/>
+      <c r="E28" s="46"/>
+      <c r="F28" s="49"/>
+      <c r="G28" s="9" t="s">
         <v>116</v>
       </c>
-      <c r="G28" s="9" t="s">
+      <c r="H28" s="9" t="s">
         <v>85</v>
       </c>
-      <c r="H28" s="9" t="s">
+      <c r="I28" s="9" t="s">
         <v>84</v>
       </c>
-      <c r="I28" s="9">
+      <c r="J28" s="9">
         <v>2</v>
       </c>
-      <c r="J28" s="11" t="s">
-        <v>40</v>
-      </c>
-      <c r="K28" s="18" t="s">
-        <v>40</v>
-      </c>
-      <c r="L28" s="51"/>
-    </row>
-    <row r="29" spans="1:13" ht="14.25" customHeight="1">
-      <c r="A29" s="45"/>
-      <c r="B29" s="45"/>
-      <c r="C29" s="48"/>
-      <c r="D29" s="48"/>
-      <c r="E29" s="45"/>
-      <c r="F29" s="9" t="s">
+      <c r="K28" s="11" t="s">
+        <v>40</v>
+      </c>
+      <c r="L28" s="18" t="s">
+        <v>40</v>
+      </c>
+      <c r="M28" s="52"/>
+    </row>
+    <row r="29" spans="1:14" ht="14.25" customHeight="1">
+      <c r="A29" s="49"/>
+      <c r="B29" s="49"/>
+      <c r="C29" s="50"/>
+      <c r="D29" s="50"/>
+      <c r="E29" s="46"/>
+      <c r="F29" s="49"/>
+      <c r="G29" s="9" t="s">
         <v>92</v>
       </c>
-      <c r="G29" s="9" t="s">
+      <c r="H29" s="9" t="s">
         <v>90</v>
       </c>
-      <c r="H29" s="9" t="s">
+      <c r="I29" s="9" t="s">
         <v>91</v>
       </c>
-      <c r="I29" s="9">
+      <c r="J29" s="9">
         <v>200</v>
       </c>
-      <c r="J29" s="11" t="s">
-        <v>40</v>
-      </c>
-      <c r="K29" s="18" t="s">
-        <v>40</v>
-      </c>
-      <c r="L29" s="51"/>
-    </row>
-    <row r="30" spans="1:13" ht="14.25" customHeight="1">
-      <c r="A30" s="45"/>
-      <c r="B30" s="45" t="s">
+      <c r="K29" s="11" t="s">
+        <v>40</v>
+      </c>
+      <c r="L29" s="18" t="s">
+        <v>40</v>
+      </c>
+      <c r="M29" s="52"/>
+    </row>
+    <row r="30" spans="1:14" ht="14.25" customHeight="1">
+      <c r="A30" s="49"/>
+      <c r="B30" s="49" t="s">
         <v>154</v>
       </c>
-      <c r="C30" s="48" t="s">
+      <c r="C30" s="50" t="s">
         <v>155</v>
       </c>
-      <c r="D30" s="48" t="s">
+      <c r="D30" s="50" t="s">
         <v>61</v>
       </c>
-      <c r="E30" s="27" t="s">
+      <c r="E30" s="46"/>
+      <c r="F30" s="27" t="s">
         <v>153</v>
       </c>
-      <c r="F30" s="9" t="s">
+      <c r="G30" s="9" t="s">
         <v>147</v>
       </c>
-      <c r="G30" s="9" t="s">
+      <c r="H30" s="9" t="s">
         <v>145</v>
       </c>
-      <c r="H30" s="9" t="s">
+      <c r="I30" s="9" t="s">
         <v>146</v>
       </c>
-      <c r="I30" s="9" t="s">
+      <c r="J30" s="9" t="s">
         <v>148</v>
       </c>
-      <c r="J30" s="11" t="s">
+      <c r="K30" s="11" t="s">
         <v>149</v>
       </c>
-      <c r="K30" s="42" t="s">
-        <v>40</v>
-      </c>
-      <c r="L30" s="51" t="s">
+      <c r="L30" s="42" t="s">
+        <v>40</v>
+      </c>
+      <c r="M30" s="52" t="s">
         <v>405</v>
       </c>
     </row>
-    <row r="31" spans="1:13" ht="14.25" customHeight="1">
-      <c r="A31" s="45"/>
-      <c r="B31" s="45"/>
-      <c r="C31" s="48"/>
-      <c r="D31" s="48"/>
-      <c r="E31" s="27" t="s">
+    <row r="31" spans="1:14" ht="14.25" customHeight="1">
+      <c r="A31" s="49"/>
+      <c r="B31" s="49"/>
+      <c r="C31" s="50"/>
+      <c r="D31" s="50"/>
+      <c r="E31" s="46"/>
+      <c r="F31" s="27" t="s">
         <v>12</v>
       </c>
-      <c r="F31" s="9" t="s">
+      <c r="G31" s="9" t="s">
         <v>150</v>
       </c>
-      <c r="G31" s="9" t="s">
+      <c r="H31" s="9" t="s">
         <v>151</v>
       </c>
-      <c r="H31" s="9" t="s">
+      <c r="I31" s="9" t="s">
         <v>146</v>
       </c>
-      <c r="I31" s="9" t="s">
+      <c r="J31" s="9" t="s">
         <v>152</v>
       </c>
-      <c r="J31" s="18" t="s">
+      <c r="K31" s="18" t="s">
         <v>149</v>
       </c>
-      <c r="K31" s="42" t="s">
-        <v>40</v>
-      </c>
-      <c r="L31" s="51"/>
-    </row>
-    <row r="32" spans="1:13" ht="14.25" customHeight="1">
-      <c r="A32" s="45"/>
-      <c r="B32" s="45"/>
-      <c r="C32" s="48"/>
-      <c r="D32" s="48"/>
-      <c r="E32" s="45" t="s">
+      <c r="L31" s="42" t="s">
+        <v>40</v>
+      </c>
+      <c r="M31" s="52"/>
+    </row>
+    <row r="32" spans="1:14" ht="14.25" customHeight="1">
+      <c r="A32" s="49"/>
+      <c r="B32" s="49"/>
+      <c r="C32" s="50"/>
+      <c r="D32" s="50"/>
+      <c r="E32" s="46"/>
+      <c r="F32" s="49" t="s">
         <v>158</v>
       </c>
-      <c r="F32" s="9" t="s">
+      <c r="G32" s="9" t="s">
         <v>144</v>
       </c>
-      <c r="G32" s="9" t="s">
+      <c r="H32" s="9" t="s">
         <v>159</v>
       </c>
-      <c r="H32" s="9" t="s">
+      <c r="I32" s="9" t="s">
         <v>146</v>
       </c>
-      <c r="I32" s="9" t="s">
+      <c r="J32" s="9" t="s">
         <v>162</v>
       </c>
-      <c r="J32" s="18" t="s">
+      <c r="K32" s="18" t="s">
         <v>149</v>
       </c>
-      <c r="K32" s="42" t="s">
-        <v>40</v>
-      </c>
-      <c r="L32" s="51"/>
-    </row>
-    <row r="33" spans="1:13" ht="14.25" customHeight="1">
-      <c r="A33" s="45"/>
-      <c r="B33" s="45"/>
-      <c r="C33" s="48"/>
-      <c r="D33" s="48"/>
-      <c r="E33" s="45"/>
-      <c r="F33" s="9" t="s">
+      <c r="L32" s="42" t="s">
+        <v>40</v>
+      </c>
+      <c r="M32" s="52"/>
+    </row>
+    <row r="33" spans="1:14" ht="14.25" customHeight="1">
+      <c r="A33" s="49"/>
+      <c r="B33" s="49"/>
+      <c r="C33" s="50"/>
+      <c r="D33" s="50"/>
+      <c r="E33" s="46"/>
+      <c r="F33" s="49"/>
+      <c r="G33" s="9" t="s">
         <v>157</v>
       </c>
-      <c r="G33" s="9" t="s">
+      <c r="H33" s="9" t="s">
         <v>160</v>
       </c>
-      <c r="H33" s="9" t="s">
+      <c r="I33" s="9" t="s">
         <v>146</v>
       </c>
-      <c r="I33" s="9" t="s">
+      <c r="J33" s="9" t="s">
         <v>163</v>
       </c>
-      <c r="J33" s="18" t="s">
+      <c r="K33" s="18" t="s">
         <v>149</v>
       </c>
-      <c r="K33" s="42" t="s">
-        <v>40</v>
-      </c>
-      <c r="L33" s="51"/>
-    </row>
-    <row r="34" spans="1:13" ht="14.25" customHeight="1">
-      <c r="A34" s="45"/>
-      <c r="B34" s="45"/>
-      <c r="C34" s="48"/>
-      <c r="D34" s="48"/>
-      <c r="E34" s="45"/>
-      <c r="F34" s="9" t="s">
+      <c r="L33" s="42" t="s">
+        <v>40</v>
+      </c>
+      <c r="M33" s="52"/>
+    </row>
+    <row r="34" spans="1:14" ht="14.25" customHeight="1">
+      <c r="A34" s="49"/>
+      <c r="B34" s="49"/>
+      <c r="C34" s="50"/>
+      <c r="D34" s="50"/>
+      <c r="E34" s="46"/>
+      <c r="F34" s="49"/>
+      <c r="G34" s="9" t="s">
         <v>156</v>
       </c>
-      <c r="G34" s="9" t="s">
+      <c r="H34" s="9" t="s">
         <v>161</v>
       </c>
-      <c r="H34" s="9" t="s">
+      <c r="I34" s="9" t="s">
         <v>146</v>
       </c>
-      <c r="I34" s="9" t="s">
+      <c r="J34" s="9" t="s">
         <v>164</v>
       </c>
-      <c r="J34" s="18" t="s">
+      <c r="K34" s="18" t="s">
         <v>149</v>
       </c>
-      <c r="K34" s="42" t="s">
-        <v>40</v>
-      </c>
-      <c r="L34" s="51"/>
-    </row>
-    <row r="35" spans="1:13" ht="57">
-      <c r="A35" s="45"/>
+      <c r="L34" s="42" t="s">
+        <v>40</v>
+      </c>
+      <c r="M34" s="52"/>
+    </row>
+    <row r="35" spans="1:14" ht="57">
+      <c r="A35" s="49"/>
       <c r="B35" s="23" t="s">
         <v>171</v>
       </c>
-      <c r="C35" s="48"/>
+      <c r="C35" s="50"/>
       <c r="D35" s="22" t="s">
         <v>170</v>
       </c>
-      <c r="E35" s="27" t="s">
+      <c r="E35" s="46"/>
+      <c r="F35" s="27" t="s">
         <v>153</v>
       </c>
-      <c r="F35" s="9" t="s">
+      <c r="G35" s="9" t="s">
         <v>46</v>
       </c>
-      <c r="G35" s="9" t="s">
+      <c r="H35" s="9" t="s">
         <v>175</v>
       </c>
-      <c r="H35" s="9" t="s">
+      <c r="I35" s="9" t="s">
         <v>169</v>
       </c>
-      <c r="I35" s="18" t="b">
+      <c r="J35" s="18" t="b">
         <v>1</v>
       </c>
-      <c r="J35" s="18" t="s">
+      <c r="K35" s="18" t="s">
         <v>201</v>
       </c>
     </row>
-    <row r="36" spans="1:13" ht="57">
-      <c r="A36" s="45"/>
+    <row r="36" spans="1:14" ht="57">
+      <c r="A36" s="49"/>
       <c r="B36" s="23" t="s">
         <v>172</v>
       </c>
-      <c r="C36" s="48"/>
+      <c r="C36" s="50"/>
       <c r="D36" s="22" t="s">
         <v>173</v>
       </c>
-      <c r="E36" s="27" t="s">
+      <c r="E36" s="46"/>
+      <c r="F36" s="27" t="s">
         <v>153</v>
       </c>
-      <c r="F36" s="9" t="s">
+      <c r="G36" s="9" t="s">
         <v>46</v>
       </c>
-      <c r="G36" s="9" t="s">
+      <c r="H36" s="9" t="s">
         <v>174</v>
       </c>
-      <c r="H36" s="9" t="s">
+      <c r="I36" s="9" t="s">
         <v>169</v>
       </c>
-      <c r="I36" s="18" t="b">
+      <c r="J36" s="18" t="b">
         <v>1</v>
       </c>
-      <c r="J36" s="18" t="s">
+      <c r="K36" s="18" t="s">
         <v>201</v>
       </c>
-      <c r="M36" s="26" t="s">
+      <c r="N36" s="26" t="s">
         <v>224</v>
       </c>
     </row>
-    <row r="37" spans="1:13" ht="28.5">
-      <c r="A37" s="45"/>
+    <row r="37" spans="1:14" ht="28.5">
+      <c r="A37" s="49"/>
       <c r="B37" s="13" t="s">
         <v>166</v>
       </c>
-      <c r="C37" s="48"/>
+      <c r="C37" s="50"/>
       <c r="D37" s="12" t="s">
         <v>143</v>
       </c>
-      <c r="E37" s="27" t="s">
+      <c r="E37" s="46"/>
+      <c r="F37" s="27" t="s">
         <v>153</v>
       </c>
-      <c r="F37" s="9" t="s">
+      <c r="G37" s="9" t="s">
         <v>153</v>
       </c>
-      <c r="J37" s="9" t="s">
-        <v>40</v>
-      </c>
       <c r="K37" s="9" t="s">
         <v>40</v>
       </c>
-      <c r="L37" s="29" t="s">
+      <c r="L37" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="M37" s="29" t="s">
         <v>317</v>
       </c>
-      <c r="M37" s="9" t="s">
+      <c r="N37" s="9" t="s">
         <v>165</v>
       </c>
     </row>
-    <row r="38" spans="1:13" ht="57" customHeight="1">
+    <row r="38" spans="1:14" ht="57" customHeight="1">
       <c r="A38" s="23"/>
-      <c r="B38" s="45" t="s">
+      <c r="B38" s="49" t="s">
         <v>167</v>
       </c>
-      <c r="C38" s="48"/>
-      <c r="D38" s="48" t="s">
+      <c r="C38" s="50"/>
+      <c r="D38" s="50" t="s">
         <v>318</v>
       </c>
-      <c r="E38" s="27" t="s">
+      <c r="E38" s="46"/>
+      <c r="F38" s="27" t="s">
         <v>153</v>
       </c>
-      <c r="F38" s="35" t="s">
+      <c r="G38" s="35" t="s">
         <v>46</v>
       </c>
-      <c r="G38" s="9" t="s">
+      <c r="H38" s="9" t="s">
         <v>168</v>
       </c>
-      <c r="H38" s="9" t="s">
+      <c r="I38" s="9" t="s">
         <v>48</v>
       </c>
-      <c r="I38" s="18" t="b">
+      <c r="J38" s="18" t="b">
         <v>1</v>
       </c>
-      <c r="J38" s="9" t="s">
-        <v>40</v>
-      </c>
       <c r="K38" s="9" t="s">
         <v>40</v>
       </c>
-      <c r="L38" s="51" t="s">
+      <c r="L38" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="M38" s="52" t="s">
         <v>398</v>
       </c>
-      <c r="M38" s="49" t="s">
+      <c r="N38" s="53" t="s">
         <v>396</v>
       </c>
     </row>
-    <row r="39" spans="1:13" s="37" customFormat="1" ht="42.75">
+    <row r="39" spans="1:14" s="37" customFormat="1" ht="42.75">
       <c r="A39" s="36"/>
-      <c r="B39" s="45"/>
-      <c r="C39" s="48"/>
-      <c r="D39" s="48"/>
-      <c r="E39" s="36" t="s">
+      <c r="B39" s="49"/>
+      <c r="C39" s="50"/>
+      <c r="D39" s="50"/>
+      <c r="E39" s="46"/>
+      <c r="F39" s="36" t="s">
         <v>319</v>
       </c>
-      <c r="F39" s="35" t="s">
+      <c r="G39" s="35" t="s">
         <v>320</v>
       </c>
-      <c r="G39" s="9" t="s">
+      <c r="H39" s="9" t="s">
         <v>59</v>
       </c>
-      <c r="H39" s="9" t="s">
+      <c r="I39" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="I39" s="26" t="s">
+      <c r="J39" s="26" t="s">
         <v>397</v>
       </c>
-      <c r="J39" s="9" t="s">
-        <v>40</v>
-      </c>
       <c r="K39" s="9" t="s">
         <v>40</v>
       </c>
-      <c r="L39" s="51"/>
-      <c r="M39" s="50"/>
-    </row>
-    <row r="40" spans="1:13" ht="28.5">
-      <c r="A40" s="45" t="s">
+      <c r="L39" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="M39" s="52"/>
+      <c r="N39" s="54"/>
+    </row>
+    <row r="40" spans="1:14" ht="28.5">
+      <c r="A40" s="49" t="s">
         <v>101</v>
       </c>
       <c r="B40" s="17" t="s">
@@ -3816,24 +3881,25 @@
       <c r="D40" s="16" t="s">
         <v>134</v>
       </c>
-      <c r="E40" s="27" t="s">
+      <c r="E40" s="46"/>
+      <c r="F40" s="27" t="s">
         <v>73</v>
-      </c>
-      <c r="J40" s="9" t="s">
-        <v>120</v>
       </c>
       <c r="K40" s="9" t="s">
         <v>120</v>
       </c>
-      <c r="L40" s="21" t="s">
+      <c r="L40" s="9" t="s">
+        <v>120</v>
+      </c>
+      <c r="M40" s="21" t="s">
         <v>135</v>
       </c>
-      <c r="M40" s="9" t="s">
+      <c r="N40" s="9" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="41" spans="1:13" ht="71.25">
-      <c r="A41" s="45"/>
+    <row r="41" spans="1:14" ht="71.25">
+      <c r="A41" s="49"/>
       <c r="B41" s="17" t="s">
         <v>210</v>
       </c>
@@ -3843,1618 +3909,1686 @@
       <c r="D41" s="16" t="s">
         <v>121</v>
       </c>
-      <c r="E41" s="27" t="s">
+      <c r="E41" s="46"/>
+      <c r="F41" s="27" t="s">
         <v>122</v>
       </c>
-      <c r="F41" s="9" t="s">
+      <c r="G41" s="9" t="s">
         <v>46</v>
       </c>
-      <c r="G41" s="9" t="s">
+      <c r="H41" s="9" t="s">
         <v>123</v>
       </c>
-      <c r="H41" s="9" t="s">
+      <c r="I41" s="9" t="s">
         <v>124</v>
       </c>
-      <c r="I41" s="18" t="b">
+      <c r="J41" s="18" t="b">
         <v>1</v>
       </c>
-      <c r="J41" s="9" t="s">
-        <v>40</v>
-      </c>
       <c r="K41" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="L41" s="9" t="s">
         <v>120</v>
       </c>
-      <c r="L41" s="21" t="s">
+      <c r="M41" s="21" t="s">
         <v>138</v>
       </c>
     </row>
-    <row r="42" spans="1:13" ht="15">
-      <c r="A42" s="45"/>
+    <row r="42" spans="1:14" ht="15">
+      <c r="A42" s="49"/>
       <c r="B42" s="44" t="s">
         <v>211</v>
       </c>
       <c r="C42" s="24"/>
       <c r="D42" s="24"/>
-      <c r="I42" s="18"/>
-      <c r="L42" s="25"/>
-    </row>
-    <row r="43" spans="1:13" ht="14.25" customHeight="1">
-      <c r="A43" s="45"/>
-      <c r="B43" s="45" t="s">
+      <c r="E42" s="46"/>
+      <c r="J42" s="18"/>
+      <c r="M42" s="25"/>
+    </row>
+    <row r="43" spans="1:14" ht="14.25" customHeight="1">
+      <c r="A43" s="49"/>
+      <c r="B43" s="49" t="s">
         <v>102</v>
       </c>
-      <c r="C43" s="48" t="s">
+      <c r="C43" s="50" t="s">
         <v>176</v>
       </c>
-      <c r="D43" s="45" t="s">
+      <c r="D43" s="49" t="s">
         <v>143</v>
       </c>
-      <c r="E43" s="45" t="s">
+      <c r="E43" s="45"/>
+      <c r="F43" s="49" t="s">
         <v>177</v>
       </c>
-      <c r="F43" s="9" t="s">
+      <c r="G43" s="9" t="s">
         <v>178</v>
       </c>
-      <c r="G43" s="9" t="s">
+      <c r="H43" s="9" t="s">
         <v>179</v>
       </c>
-      <c r="H43" s="9" t="s">
+      <c r="I43" s="9" t="s">
         <v>146</v>
       </c>
-      <c r="I43" s="9" t="s">
+      <c r="J43" s="9" t="s">
         <v>200</v>
       </c>
-      <c r="J43" s="9" t="s">
-        <v>40</v>
-      </c>
       <c r="K43" s="9" t="s">
         <v>40</v>
       </c>
-      <c r="L43" s="47" t="s">
+      <c r="L43" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="M43" s="48" t="s">
         <v>223</v>
       </c>
-      <c r="M43" s="9" t="s">
+      <c r="N43" s="9" t="s">
         <v>180</v>
       </c>
     </row>
-    <row r="44" spans="1:13">
-      <c r="A44" s="45"/>
-      <c r="B44" s="45"/>
-      <c r="C44" s="45"/>
-      <c r="D44" s="45"/>
+    <row r="44" spans="1:14">
+      <c r="A44" s="49"/>
+      <c r="B44" s="49"/>
+      <c r="C44" s="49"/>
+      <c r="D44" s="49"/>
       <c r="E44" s="45"/>
-      <c r="F44" s="18" t="s">
+      <c r="F44" s="49"/>
+      <c r="G44" s="18" t="s">
         <v>112</v>
       </c>
-      <c r="G44" s="18" t="s">
+      <c r="H44" s="18" t="s">
         <v>87</v>
       </c>
-      <c r="H44" s="18" t="s">
+      <c r="I44" s="18" t="s">
         <v>6</v>
       </c>
-      <c r="I44" s="18" t="s">
+      <c r="J44" s="18" t="s">
         <v>9</v>
       </c>
-      <c r="J44" s="9" t="s">
-        <v>40</v>
-      </c>
       <c r="K44" s="9" t="s">
         <v>40</v>
       </c>
-      <c r="L44" s="47"/>
-    </row>
-    <row r="45" spans="1:13">
-      <c r="A45" s="45"/>
-      <c r="B45" s="45"/>
-      <c r="C45" s="45"/>
-      <c r="D45" s="45"/>
+      <c r="L44" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="M44" s="48"/>
+    </row>
+    <row r="45" spans="1:14">
+      <c r="A45" s="49"/>
+      <c r="B45" s="49"/>
+      <c r="C45" s="49"/>
+      <c r="D45" s="49"/>
       <c r="E45" s="45"/>
-      <c r="F45" s="18" t="s">
+      <c r="F45" s="49"/>
+      <c r="G45" s="18" t="s">
         <v>111</v>
       </c>
-      <c r="G45" s="18" t="s">
+      <c r="H45" s="18" t="s">
         <v>74</v>
       </c>
-      <c r="H45" s="18" t="s">
+      <c r="I45" s="18" t="s">
         <v>6</v>
       </c>
-      <c r="I45" s="18" t="s">
+      <c r="J45" s="18" t="s">
         <v>77</v>
       </c>
-      <c r="J45" s="9" t="s">
-        <v>40</v>
-      </c>
       <c r="K45" s="9" t="s">
         <v>40</v>
       </c>
-      <c r="L45" s="47"/>
-    </row>
-    <row r="46" spans="1:13">
-      <c r="A46" s="45"/>
-      <c r="B46" s="45"/>
-      <c r="C46" s="45"/>
-      <c r="D46" s="45"/>
+      <c r="L45" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="M45" s="48"/>
+    </row>
+    <row r="46" spans="1:14">
+      <c r="A46" s="49"/>
+      <c r="B46" s="49"/>
+      <c r="C46" s="49"/>
+      <c r="D46" s="49"/>
       <c r="E46" s="45"/>
-      <c r="F46" s="9" t="s">
+      <c r="F46" s="49"/>
+      <c r="G46" s="9" t="s">
         <v>114</v>
       </c>
-      <c r="G46" s="18" t="s">
+      <c r="H46" s="18" t="s">
         <v>88</v>
       </c>
-      <c r="H46" s="18" t="s">
+      <c r="I46" s="18" t="s">
         <v>6</v>
       </c>
-      <c r="I46" s="18" t="s">
+      <c r="J46" s="18" t="s">
         <v>89</v>
       </c>
-      <c r="J46" s="9" t="s">
-        <v>40</v>
-      </c>
       <c r="K46" s="9" t="s">
         <v>40</v>
       </c>
-      <c r="L46" s="47"/>
-    </row>
-    <row r="47" spans="1:13">
-      <c r="A47" s="45"/>
-      <c r="B47" s="45"/>
-      <c r="C47" s="45"/>
-      <c r="D47" s="45"/>
+      <c r="L46" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="M46" s="48"/>
+    </row>
+    <row r="47" spans="1:14">
+      <c r="A47" s="49"/>
+      <c r="B47" s="49"/>
+      <c r="C47" s="49"/>
+      <c r="D47" s="49"/>
       <c r="E47" s="45"/>
-      <c r="F47" s="9" t="s">
+      <c r="F47" s="49"/>
+      <c r="G47" s="9" t="s">
         <v>113</v>
       </c>
-      <c r="G47" s="18" t="s">
+      <c r="H47" s="18" t="s">
         <v>75</v>
       </c>
-      <c r="H47" s="18" t="s">
+      <c r="I47" s="18" t="s">
         <v>6</v>
       </c>
-      <c r="I47" s="18" t="s">
+      <c r="J47" s="18" t="s">
         <v>78</v>
       </c>
-      <c r="J47" s="9" t="s">
-        <v>40</v>
-      </c>
       <c r="K47" s="9" t="s">
         <v>40</v>
       </c>
-      <c r="L47" s="47"/>
-    </row>
-    <row r="48" spans="1:13">
-      <c r="A48" s="45"/>
-      <c r="B48" s="45"/>
-      <c r="C48" s="45"/>
-      <c r="D48" s="45"/>
+      <c r="L47" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="M47" s="48"/>
+    </row>
+    <row r="48" spans="1:14">
+      <c r="A48" s="49"/>
+      <c r="B48" s="49"/>
+      <c r="C48" s="49"/>
+      <c r="D48" s="49"/>
       <c r="E48" s="45"/>
-      <c r="F48" s="9" t="s">
+      <c r="F48" s="49"/>
+      <c r="G48" s="9" t="s">
         <v>116</v>
       </c>
-      <c r="G48" s="9" t="s">
+      <c r="H48" s="9" t="s">
         <v>85</v>
       </c>
-      <c r="H48" s="9" t="s">
+      <c r="I48" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="I48" s="9">
+      <c r="J48" s="9">
         <v>2</v>
       </c>
-      <c r="J48" s="9" t="s">
-        <v>40</v>
-      </c>
       <c r="K48" s="9" t="s">
         <v>40</v>
       </c>
-      <c r="L48" s="47"/>
-    </row>
-    <row r="49" spans="1:13">
-      <c r="A49" s="45"/>
-      <c r="B49" s="45"/>
-      <c r="C49" s="45"/>
-      <c r="D49" s="45"/>
+      <c r="L48" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="M48" s="48"/>
+    </row>
+    <row r="49" spans="1:14">
+      <c r="A49" s="49"/>
+      <c r="B49" s="49"/>
+      <c r="C49" s="49"/>
+      <c r="D49" s="49"/>
       <c r="E49" s="45"/>
-      <c r="F49" s="9" t="s">
+      <c r="F49" s="49"/>
+      <c r="G49" s="9" t="s">
         <v>92</v>
       </c>
-      <c r="G49" s="9" t="s">
+      <c r="H49" s="9" t="s">
         <v>90</v>
       </c>
-      <c r="H49" s="9" t="s">
+      <c r="I49" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="I49" s="9">
+      <c r="J49" s="9">
         <v>200</v>
       </c>
-      <c r="J49" s="9" t="s">
-        <v>40</v>
-      </c>
       <c r="K49" s="9" t="s">
         <v>40</v>
       </c>
-      <c r="L49" s="47"/>
-    </row>
-    <row r="50" spans="1:13">
-      <c r="A50" s="45"/>
-      <c r="B50" s="45"/>
-      <c r="C50" s="45"/>
-      <c r="D50" s="45"/>
+      <c r="L49" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="M49" s="48"/>
+    </row>
+    <row r="50" spans="1:14">
+      <c r="A50" s="49"/>
+      <c r="B50" s="49"/>
+      <c r="C50" s="49"/>
+      <c r="D50" s="49"/>
       <c r="E50" s="45"/>
-      <c r="F50" s="9" t="s">
+      <c r="F50" s="49"/>
+      <c r="G50" s="9" t="s">
         <v>197</v>
       </c>
-      <c r="G50" s="9" t="s">
+      <c r="H50" s="9" t="s">
         <v>198</v>
       </c>
-      <c r="H50" s="9" t="s">
+      <c r="I50" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="I50" s="9" t="s">
+      <c r="J50" s="9" t="s">
         <v>199</v>
       </c>
-      <c r="J50" s="9" t="s">
-        <v>40</v>
-      </c>
       <c r="K50" s="9" t="s">
         <v>40</v>
       </c>
-      <c r="L50" s="47"/>
-    </row>
-    <row r="51" spans="1:13" ht="99.75">
-      <c r="A51" s="45"/>
-      <c r="B51" s="45"/>
-      <c r="C51" s="45"/>
-      <c r="D51" s="45"/>
+      <c r="L50" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="M50" s="48"/>
+    </row>
+    <row r="51" spans="1:14" ht="99.75">
+      <c r="A51" s="49"/>
+      <c r="B51" s="49"/>
+      <c r="C51" s="49"/>
+      <c r="D51" s="49"/>
       <c r="E51" s="45"/>
-      <c r="F51" s="9" t="s">
+      <c r="F51" s="49"/>
+      <c r="G51" s="9" t="s">
         <v>181</v>
       </c>
-      <c r="G51" s="9" t="s">
+      <c r="H51" s="9" t="s">
         <v>182</v>
       </c>
-      <c r="H51" s="9" t="s">
+      <c r="I51" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="I51" s="9" t="s">
+      <c r="J51" s="9" t="s">
         <v>183</v>
       </c>
-      <c r="J51" s="9" t="s">
-        <v>40</v>
-      </c>
       <c r="K51" s="9" t="s">
         <v>40</v>
       </c>
-      <c r="L51" s="47"/>
-      <c r="M51" s="26" t="s">
+      <c r="L51" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="M51" s="48"/>
+      <c r="N51" s="26" t="s">
         <v>404</v>
       </c>
     </row>
-    <row r="52" spans="1:13">
-      <c r="A52" s="45"/>
-      <c r="B52" s="45"/>
-      <c r="C52" s="45"/>
-      <c r="D52" s="45"/>
+    <row r="52" spans="1:14">
+      <c r="A52" s="49"/>
+      <c r="B52" s="49"/>
+      <c r="C52" s="49"/>
+      <c r="D52" s="49"/>
       <c r="E52" s="45"/>
-      <c r="F52" s="9" t="s">
+      <c r="F52" s="49"/>
+      <c r="G52" s="9" t="s">
         <v>399</v>
       </c>
-      <c r="G52" s="9" t="s">
+      <c r="H52" s="9" t="s">
         <v>400</v>
       </c>
-      <c r="H52" s="9" t="s">
+      <c r="I52" s="9" t="s">
         <v>401</v>
       </c>
-      <c r="I52" s="9" t="s">
+      <c r="J52" s="9" t="s">
         <v>402</v>
       </c>
-      <c r="J52" s="9" t="s">
+      <c r="K52" s="9" t="s">
         <v>403</v>
       </c>
-      <c r="K52" s="9" t="s">
-        <v>40</v>
-      </c>
-      <c r="L52" s="34"/>
-    </row>
-    <row r="53" spans="1:13" ht="45.75" customHeight="1">
-      <c r="A53" s="45"/>
-      <c r="B53" s="45"/>
-      <c r="C53" s="48" t="s">
+      <c r="L52" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="M52" s="34"/>
+    </row>
+    <row r="53" spans="1:14" ht="45.75" customHeight="1">
+      <c r="A53" s="49"/>
+      <c r="B53" s="49"/>
+      <c r="C53" s="50" t="s">
         <v>208</v>
       </c>
-      <c r="D53" s="48" t="s">
+      <c r="D53" s="50" t="s">
         <v>202</v>
       </c>
-      <c r="E53" s="27" t="s">
+      <c r="E53" s="46"/>
+      <c r="F53" s="27" t="s">
         <v>12</v>
       </c>
-      <c r="F53" s="9" t="s">
+      <c r="G53" s="9" t="s">
         <v>46</v>
       </c>
-      <c r="G53" s="9" t="s">
+      <c r="H53" s="9" t="s">
         <v>187</v>
       </c>
-      <c r="H53" s="9" t="s">
+      <c r="I53" s="9" t="s">
         <v>48</v>
       </c>
-      <c r="I53" s="41" t="b">
+      <c r="J53" s="41" t="b">
         <v>1</v>
       </c>
-      <c r="L53" s="47" t="s">
+      <c r="M53" s="48" t="s">
         <v>222</v>
       </c>
-      <c r="M53" s="26" t="s">
+      <c r="N53" s="26" t="s">
         <v>220</v>
       </c>
     </row>
-    <row r="54" spans="1:13">
-      <c r="A54" s="45"/>
-      <c r="B54" s="45"/>
-      <c r="C54" s="48"/>
-      <c r="D54" s="48"/>
-      <c r="E54" s="52" t="s">
+    <row r="54" spans="1:14">
+      <c r="A54" s="49"/>
+      <c r="B54" s="49"/>
+      <c r="C54" s="50"/>
+      <c r="D54" s="50"/>
+      <c r="E54" s="46"/>
+      <c r="F54" s="51" t="s">
         <v>221</v>
       </c>
-      <c r="F54" s="9" t="s">
+      <c r="G54" s="9" t="s">
         <v>213</v>
       </c>
-      <c r="G54" s="9" t="s">
+      <c r="H54" s="9" t="s">
         <v>179</v>
       </c>
-      <c r="H54" s="9" t="s">
+      <c r="I54" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="I54" s="9" t="s">
+      <c r="J54" s="9" t="s">
         <v>217</v>
-      </c>
-      <c r="J54" s="9" t="s">
-        <v>214</v>
       </c>
       <c r="K54" s="9" t="s">
         <v>214</v>
       </c>
-      <c r="L54" s="47"/>
-    </row>
-    <row r="55" spans="1:13">
-      <c r="A55" s="45"/>
-      <c r="B55" s="45"/>
-      <c r="C55" s="48"/>
-      <c r="D55" s="48"/>
-      <c r="E55" s="52"/>
-      <c r="F55" s="9" t="s">
+      <c r="L54" s="9" t="s">
+        <v>214</v>
+      </c>
+      <c r="M54" s="48"/>
+    </row>
+    <row r="55" spans="1:14">
+      <c r="A55" s="49"/>
+      <c r="B55" s="49"/>
+      <c r="C55" s="50"/>
+      <c r="D55" s="50"/>
+      <c r="E55" s="46"/>
+      <c r="F55" s="51"/>
+      <c r="G55" s="9" t="s">
         <v>215</v>
       </c>
-      <c r="G55" s="9" t="s">
+      <c r="H55" s="9" t="s">
         <v>216</v>
       </c>
-      <c r="H55" s="9" t="s">
+      <c r="I55" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="I55" s="9" t="s">
+      <c r="J55" s="9" t="s">
         <v>218</v>
-      </c>
-      <c r="J55" s="9" t="s">
-        <v>214</v>
       </c>
       <c r="K55" s="9" t="s">
         <v>214</v>
       </c>
-      <c r="L55" s="47"/>
-    </row>
-    <row r="56" spans="1:13">
-      <c r="A56" s="45"/>
-      <c r="B56" s="45"/>
-      <c r="C56" s="48"/>
-      <c r="D56" s="48"/>
-      <c r="E56" s="52"/>
-      <c r="F56" s="9" t="s">
+      <c r="L55" s="9" t="s">
+        <v>214</v>
+      </c>
+      <c r="M55" s="48"/>
+    </row>
+    <row r="56" spans="1:14">
+      <c r="A56" s="49"/>
+      <c r="B56" s="49"/>
+      <c r="C56" s="50"/>
+      <c r="D56" s="50"/>
+      <c r="E56" s="46"/>
+      <c r="F56" s="51"/>
+      <c r="G56" s="9" t="s">
         <v>203</v>
       </c>
-      <c r="G56" s="9" t="s">
+      <c r="H56" s="9" t="s">
         <v>204</v>
       </c>
-      <c r="H56" s="9" t="s">
+      <c r="I56" s="9" t="s">
         <v>205</v>
       </c>
-      <c r="I56" s="9" t="s">
+      <c r="J56" s="9" t="s">
         <v>199</v>
-      </c>
-      <c r="J56" s="9" t="s">
-        <v>214</v>
       </c>
       <c r="K56" s="9" t="s">
         <v>214</v>
       </c>
-      <c r="L56" s="47"/>
-    </row>
-    <row r="57" spans="1:13">
-      <c r="A57" s="45"/>
-      <c r="B57" s="45"/>
-      <c r="C57" s="48"/>
-      <c r="D57" s="48"/>
-      <c r="E57" s="52"/>
-      <c r="F57" s="9" t="s">
+      <c r="L56" s="9" t="s">
+        <v>214</v>
+      </c>
+      <c r="M56" s="48"/>
+    </row>
+    <row r="57" spans="1:14">
+      <c r="A57" s="49"/>
+      <c r="B57" s="49"/>
+      <c r="C57" s="50"/>
+      <c r="D57" s="50"/>
+      <c r="E57" s="46"/>
+      <c r="F57" s="51"/>
+      <c r="G57" s="9" t="s">
         <v>219</v>
       </c>
-      <c r="G57" s="9" t="s">
+      <c r="H57" s="9" t="s">
         <v>206</v>
       </c>
-      <c r="H57" s="9" t="s">
+      <c r="I57" s="9" t="s">
         <v>205</v>
       </c>
-      <c r="I57" s="9" t="s">
+      <c r="J57" s="9" t="s">
         <v>207</v>
-      </c>
-      <c r="J57" s="9" t="s">
-        <v>214</v>
       </c>
       <c r="K57" s="9" t="s">
         <v>214</v>
       </c>
-      <c r="L57" s="47"/>
-    </row>
-    <row r="58" spans="1:13">
-      <c r="A58" s="45"/>
-      <c r="B58" s="45" t="s">
+      <c r="L57" s="9" t="s">
+        <v>214</v>
+      </c>
+      <c r="M57" s="48"/>
+    </row>
+    <row r="58" spans="1:14">
+      <c r="A58" s="49"/>
+      <c r="B58" s="49" t="s">
         <v>184</v>
       </c>
-      <c r="C58" s="48" t="s">
+      <c r="C58" s="50" t="s">
         <v>185</v>
       </c>
-      <c r="D58" s="48" t="s">
+      <c r="D58" s="50" t="s">
         <v>194</v>
       </c>
-      <c r="E58" s="27" t="s">
+      <c r="E58" s="46"/>
+      <c r="F58" s="27" t="s">
         <v>153</v>
       </c>
-      <c r="F58" s="9" t="s">
+      <c r="G58" s="9" t="s">
         <v>186</v>
       </c>
-      <c r="G58" s="9" t="s">
+      <c r="H58" s="9" t="s">
         <v>187</v>
       </c>
-      <c r="H58" s="9" t="s">
+      <c r="I58" s="9" t="s">
         <v>169</v>
       </c>
-      <c r="I58" s="18" t="b">
+      <c r="J58" s="18" t="b">
         <v>1</v>
       </c>
-      <c r="J58" s="9" t="s">
-        <v>40</v>
-      </c>
       <c r="K58" s="9" t="s">
         <v>40</v>
       </c>
-      <c r="L58" s="46" t="s">
-        <v>427</v>
-      </c>
-      <c r="M58" s="9" t="s">
+      <c r="L58" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="M58" s="47" t="s">
+        <v>426</v>
+      </c>
+      <c r="N58" s="9" t="s">
         <v>188</v>
       </c>
     </row>
-    <row r="59" spans="1:13">
-      <c r="A59" s="45"/>
-      <c r="B59" s="45"/>
-      <c r="C59" s="48"/>
-      <c r="D59" s="48"/>
-      <c r="E59" s="45" t="s">
+    <row r="59" spans="1:14">
+      <c r="A59" s="49"/>
+      <c r="B59" s="49"/>
+      <c r="C59" s="50"/>
+      <c r="D59" s="50"/>
+      <c r="E59" s="46"/>
+      <c r="F59" s="49" t="s">
         <v>195</v>
       </c>
-      <c r="F59" s="9" t="s">
+      <c r="G59" s="9" t="s">
         <v>144</v>
       </c>
-      <c r="G59" s="9" t="s">
+      <c r="H59" s="9" t="s">
         <v>159</v>
       </c>
-      <c r="H59" s="9" t="s">
+      <c r="I59" s="9" t="s">
         <v>146</v>
       </c>
-      <c r="I59" s="9" t="s">
+      <c r="J59" s="9" t="s">
         <v>162</v>
       </c>
-      <c r="J59" s="9" t="s">
-        <v>40</v>
-      </c>
       <c r="K59" s="9" t="s">
         <v>40</v>
       </c>
-      <c r="L59" s="47"/>
-      <c r="M59" s="9" t="s">
+      <c r="L59" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="M59" s="48"/>
+      <c r="N59" s="9" t="s">
         <v>196</v>
       </c>
     </row>
-    <row r="60" spans="1:13">
-      <c r="A60" s="45"/>
-      <c r="B60" s="45"/>
-      <c r="C60" s="48"/>
-      <c r="D60" s="48"/>
-      <c r="E60" s="45"/>
-      <c r="F60" s="9" t="s">
+    <row r="60" spans="1:14">
+      <c r="A60" s="49"/>
+      <c r="B60" s="49"/>
+      <c r="C60" s="50"/>
+      <c r="D60" s="50"/>
+      <c r="E60" s="46"/>
+      <c r="F60" s="49"/>
+      <c r="G60" s="9" t="s">
         <v>157</v>
       </c>
-      <c r="G60" s="9" t="s">
+      <c r="H60" s="9" t="s">
         <v>160</v>
       </c>
-      <c r="H60" s="9" t="s">
+      <c r="I60" s="9" t="s">
         <v>146</v>
       </c>
-      <c r="I60" s="9" t="s">
+      <c r="J60" s="9" t="s">
         <v>163</v>
       </c>
-      <c r="J60" s="9" t="s">
-        <v>40</v>
-      </c>
       <c r="K60" s="9" t="s">
         <v>40</v>
       </c>
-      <c r="L60" s="47"/>
-    </row>
-    <row r="61" spans="1:13">
-      <c r="A61" s="45"/>
-      <c r="B61" s="45"/>
-      <c r="C61" s="48"/>
-      <c r="D61" s="48"/>
-      <c r="E61" s="45"/>
-      <c r="F61" s="9" t="s">
+      <c r="L60" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="M60" s="48"/>
+    </row>
+    <row r="61" spans="1:14">
+      <c r="A61" s="49"/>
+      <c r="B61" s="49"/>
+      <c r="C61" s="50"/>
+      <c r="D61" s="50"/>
+      <c r="E61" s="46"/>
+      <c r="F61" s="49"/>
+      <c r="G61" s="9" t="s">
         <v>189</v>
       </c>
-      <c r="G61" s="9" t="s">
+      <c r="H61" s="9" t="s">
         <v>190</v>
       </c>
-      <c r="H61" s="9" t="s">
+      <c r="I61" s="9" t="s">
         <v>146</v>
       </c>
-      <c r="I61" s="9" t="s">
+      <c r="J61" s="9" t="s">
         <v>32</v>
       </c>
-      <c r="J61" s="9" t="s">
-        <v>40</v>
-      </c>
       <c r="K61" s="9" t="s">
         <v>40</v>
       </c>
-      <c r="L61" s="47"/>
-    </row>
-    <row r="62" spans="1:13">
-      <c r="A62" s="45"/>
-      <c r="B62" s="45"/>
-      <c r="C62" s="48"/>
-      <c r="D62" s="48"/>
-      <c r="E62" s="45"/>
-      <c r="F62" s="9" t="s">
+      <c r="L61" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="M61" s="48"/>
+    </row>
+    <row r="62" spans="1:14">
+      <c r="A62" s="49"/>
+      <c r="B62" s="49"/>
+      <c r="C62" s="50"/>
+      <c r="D62" s="50"/>
+      <c r="E62" s="46"/>
+      <c r="F62" s="49"/>
+      <c r="G62" s="9" t="s">
         <v>191</v>
       </c>
-      <c r="G62" s="9" t="s">
+      <c r="H62" s="9" t="s">
         <v>192</v>
       </c>
-      <c r="H62" s="9" t="s">
+      <c r="I62" s="9" t="s">
         <v>146</v>
       </c>
-      <c r="I62" s="9" t="s">
+      <c r="J62" s="9" t="s">
         <v>193</v>
       </c>
-      <c r="J62" s="9" t="s">
-        <v>40</v>
-      </c>
       <c r="K62" s="9" t="s">
         <v>40</v>
       </c>
-      <c r="L62" s="47"/>
-    </row>
-    <row r="63" spans="1:13">
-      <c r="A63" s="45" t="s">
+      <c r="L62" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="M62" s="48"/>
+    </row>
+    <row r="63" spans="1:14">
+      <c r="A63" s="49" t="s">
         <v>103</v>
       </c>
-      <c r="B63" s="45" t="s">
+      <c r="B63" s="49" t="s">
         <v>104</v>
       </c>
-      <c r="C63" s="45" t="s">
+      <c r="C63" s="49" t="s">
         <v>209</v>
       </c>
-      <c r="D63" s="45" t="s">
+      <c r="D63" s="49" t="s">
         <v>225</v>
       </c>
-      <c r="E63" s="45" t="s">
+      <c r="E63" s="45"/>
+      <c r="F63" s="49" t="s">
         <v>300</v>
       </c>
-      <c r="F63" s="9" t="s">
+      <c r="G63" s="9" t="s">
         <v>226</v>
       </c>
-      <c r="G63" s="9" t="s">
+      <c r="H63" s="9" t="s">
         <v>227</v>
       </c>
-      <c r="H63" s="9" t="s">
+      <c r="I63" s="9" t="s">
         <v>228</v>
       </c>
-      <c r="I63" s="9" t="s">
+      <c r="J63" s="9" t="s">
         <v>230</v>
       </c>
-      <c r="J63" s="9" t="s">
-        <v>40</v>
-      </c>
       <c r="K63" s="9" t="s">
         <v>40</v>
       </c>
-      <c r="L63" s="46" t="s">
+      <c r="L63" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="M63" s="47" t="s">
         <v>316</v>
       </c>
     </row>
-    <row r="64" spans="1:13">
-      <c r="A64" s="45"/>
-      <c r="B64" s="45"/>
-      <c r="C64" s="45"/>
-      <c r="D64" s="45"/>
+    <row r="64" spans="1:14">
+      <c r="A64" s="49"/>
+      <c r="B64" s="49"/>
+      <c r="C64" s="49"/>
+      <c r="D64" s="49"/>
       <c r="E64" s="45"/>
-      <c r="F64" s="9" t="s">
+      <c r="F64" s="49"/>
+      <c r="G64" s="9" t="s">
         <v>231</v>
       </c>
-      <c r="G64" s="9" t="s">
+      <c r="H64" s="9" t="s">
         <v>237</v>
       </c>
-      <c r="H64" s="9" t="s">
+      <c r="I64" s="9" t="s">
         <v>228</v>
       </c>
-      <c r="I64" s="9" t="s">
+      <c r="J64" s="9" t="s">
         <v>238</v>
       </c>
-      <c r="J64" s="9" t="s">
-        <v>40</v>
-      </c>
       <c r="K64" s="9" t="s">
         <v>40</v>
       </c>
-      <c r="L64" s="47"/>
-    </row>
-    <row r="65" spans="1:13">
-      <c r="A65" s="45"/>
-      <c r="B65" s="45"/>
-      <c r="C65" s="45"/>
-      <c r="D65" s="45"/>
+      <c r="L64" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="M64" s="48"/>
+    </row>
+    <row r="65" spans="1:14">
+      <c r="A65" s="49"/>
+      <c r="B65" s="49"/>
+      <c r="C65" s="49"/>
+      <c r="D65" s="49"/>
       <c r="E65" s="45"/>
-      <c r="F65" s="9" t="s">
+      <c r="F65" s="49"/>
+      <c r="G65" s="9" t="s">
         <v>232</v>
       </c>
-      <c r="G65" s="9" t="s">
+      <c r="H65" s="9" t="s">
         <v>239</v>
       </c>
-      <c r="H65" s="9" t="s">
+      <c r="I65" s="9" t="s">
         <v>228</v>
       </c>
-      <c r="I65" s="9" t="s">
+      <c r="J65" s="9" t="s">
         <v>240</v>
       </c>
-      <c r="J65" s="9" t="s">
-        <v>40</v>
-      </c>
       <c r="K65" s="9" t="s">
         <v>40</v>
       </c>
-      <c r="L65" s="47"/>
-    </row>
-    <row r="66" spans="1:13">
-      <c r="A66" s="45"/>
-      <c r="B66" s="45"/>
-      <c r="C66" s="45"/>
-      <c r="D66" s="45"/>
+      <c r="L65" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="M65" s="48"/>
+    </row>
+    <row r="66" spans="1:14">
+      <c r="A66" s="49"/>
+      <c r="B66" s="49"/>
+      <c r="C66" s="49"/>
+      <c r="D66" s="49"/>
       <c r="E66" s="45"/>
-      <c r="F66" s="9" t="s">
+      <c r="F66" s="49"/>
+      <c r="G66" s="9" t="s">
         <v>233</v>
       </c>
-      <c r="G66" s="9" t="s">
+      <c r="H66" s="9" t="s">
         <v>241</v>
       </c>
-      <c r="H66" s="9" t="s">
+      <c r="I66" s="9" t="s">
         <v>228</v>
       </c>
-      <c r="I66" s="9" t="s">
+      <c r="J66" s="9" t="s">
         <v>229</v>
       </c>
-      <c r="J66" s="9" t="s">
-        <v>40</v>
-      </c>
       <c r="K66" s="9" t="s">
         <v>40</v>
       </c>
-      <c r="L66" s="47"/>
-    </row>
-    <row r="67" spans="1:13">
-      <c r="A67" s="45"/>
-      <c r="B67" s="45"/>
-      <c r="C67" s="45"/>
-      <c r="D67" s="45"/>
+      <c r="L66" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="M66" s="48"/>
+    </row>
+    <row r="67" spans="1:14">
+      <c r="A67" s="49"/>
+      <c r="B67" s="49"/>
+      <c r="C67" s="49"/>
+      <c r="D67" s="49"/>
       <c r="E67" s="45"/>
-      <c r="F67" s="9" t="s">
+      <c r="F67" s="49"/>
+      <c r="G67" s="9" t="s">
         <v>234</v>
       </c>
-      <c r="G67" s="9" t="s">
+      <c r="H67" s="9" t="s">
         <v>242</v>
       </c>
-      <c r="H67" s="9" t="s">
+      <c r="I67" s="9" t="s">
         <v>228</v>
       </c>
-      <c r="I67" s="9" t="s">
+      <c r="J67" s="9" t="s">
         <v>243</v>
       </c>
-      <c r="J67" s="9" t="s">
-        <v>40</v>
-      </c>
       <c r="K67" s="9" t="s">
         <v>40</v>
       </c>
-      <c r="L67" s="47"/>
-    </row>
-    <row r="68" spans="1:13">
-      <c r="A68" s="45"/>
-      <c r="B68" s="45"/>
-      <c r="C68" s="45"/>
-      <c r="D68" s="45"/>
+      <c r="L67" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="M67" s="48"/>
+    </row>
+    <row r="68" spans="1:14">
+      <c r="A68" s="49"/>
+      <c r="B68" s="49"/>
+      <c r="C68" s="49"/>
+      <c r="D68" s="49"/>
       <c r="E68" s="45"/>
-      <c r="F68" s="9" t="s">
+      <c r="F68" s="49"/>
+      <c r="G68" s="9" t="s">
         <v>244</v>
       </c>
-      <c r="G68" s="9" t="s">
+      <c r="H68" s="9" t="s">
         <v>245</v>
       </c>
-      <c r="H68" s="9" t="s">
+      <c r="I68" s="9" t="s">
         <v>228</v>
       </c>
-      <c r="I68" s="9" t="s">
+      <c r="J68" s="9" t="s">
         <v>246</v>
       </c>
-      <c r="J68" s="9" t="s">
-        <v>40</v>
-      </c>
       <c r="K68" s="9" t="s">
         <v>40</v>
       </c>
-      <c r="L68" s="47"/>
-    </row>
-    <row r="69" spans="1:13">
-      <c r="A69" s="45"/>
-      <c r="B69" s="45"/>
-      <c r="C69" s="45"/>
-      <c r="D69" s="45"/>
+      <c r="L68" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="M68" s="48"/>
+    </row>
+    <row r="69" spans="1:14">
+      <c r="A69" s="49"/>
+      <c r="B69" s="49"/>
+      <c r="C69" s="49"/>
+      <c r="D69" s="49"/>
       <c r="E69" s="45"/>
-      <c r="F69" s="9" t="s">
+      <c r="F69" s="49"/>
+      <c r="G69" s="9" t="s">
         <v>235</v>
       </c>
-      <c r="G69" s="9" t="s">
+      <c r="H69" s="9" t="s">
         <v>247</v>
       </c>
-      <c r="H69" s="9" t="s">
+      <c r="I69" s="9" t="s">
         <v>228</v>
       </c>
-      <c r="I69" s="9" t="s">
+      <c r="J69" s="9" t="s">
         <v>249</v>
       </c>
-      <c r="J69" s="9" t="s">
-        <v>40</v>
-      </c>
       <c r="K69" s="9" t="s">
         <v>40</v>
       </c>
-      <c r="L69" s="47"/>
-    </row>
-    <row r="70" spans="1:13">
-      <c r="A70" s="45"/>
-      <c r="B70" s="45"/>
-      <c r="C70" s="45"/>
-      <c r="D70" s="45"/>
+      <c r="L69" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="M69" s="48"/>
+    </row>
+    <row r="70" spans="1:14">
+      <c r="A70" s="49"/>
+      <c r="B70" s="49"/>
+      <c r="C70" s="49"/>
+      <c r="D70" s="49"/>
       <c r="E70" s="45"/>
-      <c r="F70" s="9" t="s">
+      <c r="F70" s="49"/>
+      <c r="G70" s="9" t="s">
         <v>236</v>
       </c>
-      <c r="G70" s="9" t="s">
+      <c r="H70" s="9" t="s">
         <v>248</v>
       </c>
-      <c r="H70" s="9" t="s">
+      <c r="I70" s="9" t="s">
         <v>228</v>
       </c>
-      <c r="I70" s="9" t="s">
+      <c r="J70" s="9" t="s">
         <v>250</v>
       </c>
-      <c r="J70" s="9" t="s">
-        <v>40</v>
-      </c>
       <c r="K70" s="9" t="s">
         <v>40</v>
       </c>
-      <c r="L70" s="47"/>
-    </row>
-    <row r="71" spans="1:13">
-      <c r="A71" s="45"/>
-      <c r="B71" s="45"/>
-      <c r="C71" s="45"/>
-      <c r="D71" s="45"/>
+      <c r="L70" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="M70" s="48"/>
+    </row>
+    <row r="71" spans="1:14">
+      <c r="A71" s="49"/>
+      <c r="B71" s="49"/>
+      <c r="C71" s="49"/>
+      <c r="D71" s="49"/>
       <c r="E71" s="45"/>
-      <c r="F71" s="9" t="s">
+      <c r="F71" s="49"/>
+      <c r="G71" s="9" t="s">
         <v>251</v>
       </c>
-      <c r="G71" s="9" t="s">
+      <c r="H71" s="9" t="s">
         <v>252</v>
       </c>
-      <c r="H71" s="9" t="s">
+      <c r="I71" s="9" t="s">
         <v>228</v>
       </c>
-      <c r="I71" s="9" t="s">
+      <c r="J71" s="9" t="s">
         <v>301</v>
       </c>
-      <c r="J71" s="9" t="s">
-        <v>40</v>
-      </c>
       <c r="K71" s="9" t="s">
         <v>40</v>
       </c>
-      <c r="L71" s="47"/>
-    </row>
-    <row r="72" spans="1:13">
-      <c r="A72" s="45"/>
-      <c r="B72" s="45"/>
-      <c r="C72" s="45"/>
-      <c r="D72" s="45"/>
+      <c r="L71" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="M71" s="48"/>
+    </row>
+    <row r="72" spans="1:14">
+      <c r="A72" s="49"/>
+      <c r="B72" s="49"/>
+      <c r="C72" s="49"/>
+      <c r="D72" s="49"/>
       <c r="E72" s="45"/>
-      <c r="F72" s="9" t="s">
+      <c r="F72" s="49"/>
+      <c r="G72" s="9" t="s">
         <v>265</v>
       </c>
-      <c r="G72" s="9" t="s">
+      <c r="H72" s="9" t="s">
         <v>253</v>
       </c>
-      <c r="H72" s="9" t="s">
+      <c r="I72" s="9" t="s">
         <v>228</v>
       </c>
-      <c r="I72" s="9" t="s">
+      <c r="J72" s="9" t="s">
         <v>254</v>
       </c>
-      <c r="J72" s="9" t="s">
-        <v>40</v>
-      </c>
       <c r="K72" s="9" t="s">
         <v>40</v>
       </c>
-      <c r="L72" s="47"/>
-    </row>
-    <row r="73" spans="1:13" s="3" customFormat="1">
-      <c r="A73" s="45"/>
-      <c r="B73" s="45"/>
-      <c r="C73" s="45"/>
-      <c r="D73" s="45"/>
+      <c r="L72" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="M72" s="48"/>
+    </row>
+    <row r="73" spans="1:14" s="3" customFormat="1">
+      <c r="A73" s="49"/>
+      <c r="B73" s="49"/>
+      <c r="C73" s="49"/>
+      <c r="D73" s="49"/>
       <c r="E73" s="45"/>
-      <c r="F73" s="28" t="s">
+      <c r="F73" s="49"/>
+      <c r="G73" s="28" t="s">
         <v>256</v>
       </c>
-      <c r="G73" s="28" t="s">
+      <c r="H73" s="28" t="s">
         <v>257</v>
       </c>
-      <c r="H73" s="28" t="s">
+      <c r="I73" s="28" t="s">
         <v>228</v>
       </c>
-      <c r="I73" s="28" t="s">
+      <c r="J73" s="28" t="s">
         <v>302</v>
       </c>
-      <c r="J73" s="9" t="s">
-        <v>40</v>
-      </c>
       <c r="K73" s="9" t="s">
         <v>40</v>
       </c>
-      <c r="L73" s="47"/>
-      <c r="M73" s="28"/>
-    </row>
-    <row r="74" spans="1:13">
-      <c r="A74" s="45"/>
-      <c r="B74" s="45"/>
-      <c r="C74" s="45"/>
-      <c r="D74" s="45"/>
+      <c r="L73" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="M73" s="48"/>
+      <c r="N73" s="28"/>
+    </row>
+    <row r="74" spans="1:14">
+      <c r="A74" s="49"/>
+      <c r="B74" s="49"/>
+      <c r="C74" s="49"/>
+      <c r="D74" s="49"/>
       <c r="E74" s="45"/>
-      <c r="F74" s="9" t="s">
+      <c r="F74" s="49"/>
+      <c r="G74" s="9" t="s">
         <v>258</v>
       </c>
-      <c r="G74" s="9" t="s">
+      <c r="H74" s="9" t="s">
         <v>259</v>
       </c>
-      <c r="H74" s="9" t="s">
+      <c r="I74" s="9" t="s">
         <v>228</v>
       </c>
-      <c r="I74" s="9" t="s">
+      <c r="J74" s="9" t="s">
         <v>229</v>
       </c>
-      <c r="J74" s="9" t="s">
-        <v>40</v>
-      </c>
       <c r="K74" s="9" t="s">
         <v>40</v>
       </c>
-      <c r="L74" s="47"/>
-    </row>
-    <row r="75" spans="1:13">
-      <c r="A75" s="45"/>
-      <c r="B75" s="45"/>
-      <c r="C75" s="45"/>
-      <c r="D75" s="45"/>
+      <c r="L74" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="M74" s="48"/>
+    </row>
+    <row r="75" spans="1:14">
+      <c r="A75" s="49"/>
+      <c r="B75" s="49"/>
+      <c r="C75" s="49"/>
+      <c r="D75" s="49"/>
       <c r="E75" s="45"/>
-      <c r="F75" s="9" t="s">
+      <c r="F75" s="49"/>
+      <c r="G75" s="9" t="s">
         <v>260</v>
       </c>
-      <c r="G75" s="9" t="s">
+      <c r="H75" s="9" t="s">
         <v>261</v>
       </c>
-      <c r="H75" s="9" t="s">
+      <c r="I75" s="9" t="s">
         <v>262</v>
       </c>
-      <c r="I75" s="9" t="s">
+      <c r="J75" s="9" t="s">
         <v>308</v>
       </c>
-      <c r="J75" s="9" t="s">
-        <v>40</v>
-      </c>
       <c r="K75" s="9" t="s">
         <v>40</v>
       </c>
-      <c r="L75" s="47"/>
-    </row>
-    <row r="76" spans="1:13">
-      <c r="A76" s="45"/>
-      <c r="B76" s="45"/>
-      <c r="C76" s="45"/>
-      <c r="D76" s="45"/>
+      <c r="L75" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="M75" s="48"/>
+    </row>
+    <row r="76" spans="1:14">
+      <c r="A76" s="49"/>
+      <c r="B76" s="49"/>
+      <c r="C76" s="49"/>
+      <c r="D76" s="49"/>
       <c r="E76" s="45"/>
-      <c r="F76" s="9" t="s">
+      <c r="F76" s="49"/>
+      <c r="G76" s="9" t="s">
         <v>263</v>
       </c>
-      <c r="G76" s="9" t="s">
+      <c r="H76" s="9" t="s">
         <v>264</v>
       </c>
-      <c r="H76" s="9" t="s">
+      <c r="I76" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="I76" s="9" t="s">
+      <c r="J76" s="9" t="s">
         <v>229</v>
       </c>
-      <c r="J76" s="9" t="s">
-        <v>40</v>
-      </c>
       <c r="K76" s="9" t="s">
         <v>40</v>
       </c>
-      <c r="L76" s="47"/>
-    </row>
-    <row r="77" spans="1:13">
-      <c r="A77" s="45"/>
-      <c r="B77" s="45"/>
-      <c r="C77" s="45"/>
-      <c r="D77" s="45"/>
+      <c r="L76" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="M76" s="48"/>
+    </row>
+    <row r="77" spans="1:14">
+      <c r="A77" s="49"/>
+      <c r="B77" s="49"/>
+      <c r="C77" s="49"/>
+      <c r="D77" s="49"/>
       <c r="E77" s="45"/>
-      <c r="F77" s="9" t="s">
+      <c r="F77" s="49"/>
+      <c r="G77" s="9" t="s">
         <v>266</v>
       </c>
-      <c r="G77" s="9" t="s">
+      <c r="H77" s="9" t="s">
         <v>284</v>
       </c>
-      <c r="H77" s="9" t="s">
+      <c r="I77" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="I77" s="9" t="s">
+      <c r="J77" s="9" t="s">
         <v>303</v>
       </c>
-      <c r="J77" s="9" t="s">
-        <v>40</v>
-      </c>
       <c r="K77" s="9" t="s">
         <v>40</v>
       </c>
-      <c r="L77" s="47"/>
-    </row>
-    <row r="78" spans="1:13">
-      <c r="A78" s="45"/>
-      <c r="B78" s="45"/>
-      <c r="C78" s="45"/>
-      <c r="D78" s="45"/>
+      <c r="L77" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="M77" s="48"/>
+    </row>
+    <row r="78" spans="1:14">
+      <c r="A78" s="49"/>
+      <c r="B78" s="49"/>
+      <c r="C78" s="49"/>
+      <c r="D78" s="49"/>
       <c r="E78" s="45"/>
-      <c r="F78" s="9" t="s">
+      <c r="F78" s="49"/>
+      <c r="G78" s="9" t="s">
         <v>267</v>
       </c>
-      <c r="G78" s="9" t="s">
+      <c r="H78" s="9" t="s">
         <v>285</v>
       </c>
-      <c r="H78" s="9" t="s">
+      <c r="I78" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="I78" s="9" t="s">
+      <c r="J78" s="9" t="s">
         <v>303</v>
       </c>
-      <c r="J78" s="9" t="s">
-        <v>40</v>
-      </c>
       <c r="K78" s="9" t="s">
         <v>40</v>
       </c>
-      <c r="L78" s="47"/>
-    </row>
-    <row r="79" spans="1:13">
-      <c r="A79" s="45"/>
-      <c r="B79" s="45"/>
-      <c r="C79" s="45"/>
-      <c r="D79" s="45"/>
+      <c r="L78" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="M78" s="48"/>
+    </row>
+    <row r="79" spans="1:14">
+      <c r="A79" s="49"/>
+      <c r="B79" s="49"/>
+      <c r="C79" s="49"/>
+      <c r="D79" s="49"/>
       <c r="E79" s="45"/>
-      <c r="F79" s="9" t="s">
+      <c r="F79" s="49"/>
+      <c r="G79" s="9" t="s">
         <v>268</v>
       </c>
-      <c r="G79" s="9" t="s">
+      <c r="H79" s="9" t="s">
         <v>286</v>
       </c>
-      <c r="H79" s="9" t="s">
+      <c r="I79" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="I79" s="9" t="s">
+      <c r="J79" s="9" t="s">
         <v>304</v>
       </c>
-      <c r="J79" s="9" t="s">
-        <v>40</v>
-      </c>
       <c r="K79" s="9" t="s">
         <v>40</v>
       </c>
-      <c r="L79" s="47"/>
-    </row>
-    <row r="80" spans="1:13">
-      <c r="A80" s="45"/>
-      <c r="B80" s="45"/>
-      <c r="C80" s="45"/>
-      <c r="D80" s="45"/>
+      <c r="L79" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="M79" s="48"/>
+    </row>
+    <row r="80" spans="1:14">
+      <c r="A80" s="49"/>
+      <c r="B80" s="49"/>
+      <c r="C80" s="49"/>
+      <c r="D80" s="49"/>
       <c r="E80" s="45"/>
-      <c r="F80" s="9" t="s">
+      <c r="F80" s="49"/>
+      <c r="G80" s="9" t="s">
         <v>269</v>
       </c>
-      <c r="G80" s="9" t="s">
+      <c r="H80" s="9" t="s">
         <v>287</v>
       </c>
-      <c r="H80" s="9" t="s">
+      <c r="I80" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="I80" s="9" t="s">
+      <c r="J80" s="9" t="s">
         <v>305</v>
       </c>
-      <c r="J80" s="9" t="s">
-        <v>40</v>
-      </c>
       <c r="K80" s="9" t="s">
         <v>40</v>
       </c>
-      <c r="L80" s="47"/>
-    </row>
-    <row r="81" spans="1:12">
-      <c r="A81" s="45"/>
-      <c r="B81" s="45"/>
-      <c r="C81" s="45"/>
-      <c r="D81" s="45"/>
+      <c r="L80" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="M80" s="48"/>
+    </row>
+    <row r="81" spans="1:13">
+      <c r="A81" s="49"/>
+      <c r="B81" s="49"/>
+      <c r="C81" s="49"/>
+      <c r="D81" s="49"/>
       <c r="E81" s="45"/>
-      <c r="F81" s="9" t="s">
+      <c r="F81" s="49"/>
+      <c r="G81" s="9" t="s">
         <v>270</v>
       </c>
-      <c r="G81" s="9" t="s">
+      <c r="H81" s="9" t="s">
         <v>288</v>
       </c>
-      <c r="H81" s="9" t="s">
+      <c r="I81" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="I81" s="9" t="s">
+      <c r="J81" s="9" t="s">
         <v>306</v>
       </c>
-      <c r="J81" s="9" t="s">
-        <v>40</v>
-      </c>
       <c r="K81" s="9" t="s">
         <v>40</v>
       </c>
-      <c r="L81" s="47"/>
-    </row>
-    <row r="82" spans="1:12">
-      <c r="A82" s="45"/>
-      <c r="B82" s="45"/>
-      <c r="C82" s="45"/>
-      <c r="D82" s="45"/>
+      <c r="L81" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="M81" s="48"/>
+    </row>
+    <row r="82" spans="1:13">
+      <c r="A82" s="49"/>
+      <c r="B82" s="49"/>
+      <c r="C82" s="49"/>
+      <c r="D82" s="49"/>
       <c r="E82" s="45"/>
-      <c r="F82" s="9" t="s">
+      <c r="F82" s="49"/>
+      <c r="G82" s="9" t="s">
         <v>271</v>
       </c>
-      <c r="G82" s="9" t="s">
+      <c r="H82" s="9" t="s">
         <v>289</v>
       </c>
-      <c r="H82" s="9" t="s">
+      <c r="I82" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="I82" s="9" t="s">
+      <c r="J82" s="9" t="s">
         <v>307</v>
       </c>
-      <c r="J82" s="9" t="s">
-        <v>40</v>
-      </c>
       <c r="K82" s="9" t="s">
         <v>40</v>
       </c>
-      <c r="L82" s="47"/>
-    </row>
-    <row r="83" spans="1:12">
-      <c r="A83" s="45"/>
-      <c r="B83" s="45"/>
-      <c r="C83" s="45"/>
-      <c r="D83" s="45"/>
+      <c r="L82" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="M82" s="48"/>
+    </row>
+    <row r="83" spans="1:13">
+      <c r="A83" s="49"/>
+      <c r="B83" s="49"/>
+      <c r="C83" s="49"/>
+      <c r="D83" s="49"/>
       <c r="E83" s="45"/>
-      <c r="F83" s="9" t="s">
+      <c r="F83" s="49"/>
+      <c r="G83" s="9" t="s">
         <v>272</v>
       </c>
-      <c r="G83" s="9" t="s">
+      <c r="H83" s="9" t="s">
         <v>290</v>
       </c>
-      <c r="H83" s="9" t="s">
+      <c r="I83" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="I83" s="9" t="s">
+      <c r="J83" s="9" t="s">
         <v>309</v>
       </c>
-      <c r="J83" s="9" t="s">
-        <v>40</v>
-      </c>
       <c r="K83" s="9" t="s">
         <v>40</v>
       </c>
-      <c r="L83" s="47"/>
-    </row>
-    <row r="84" spans="1:12">
-      <c r="A84" s="45"/>
-      <c r="B84" s="45"/>
-      <c r="C84" s="45"/>
-      <c r="D84" s="45"/>
+      <c r="L83" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="M83" s="48"/>
+    </row>
+    <row r="84" spans="1:13">
+      <c r="A84" s="49"/>
+      <c r="B84" s="49"/>
+      <c r="C84" s="49"/>
+      <c r="D84" s="49"/>
       <c r="E84" s="45"/>
-      <c r="F84" s="9" t="s">
+      <c r="F84" s="49"/>
+      <c r="G84" s="9" t="s">
         <v>273</v>
       </c>
-      <c r="G84" s="9" t="s">
+      <c r="H84" s="9" t="s">
         <v>291</v>
       </c>
-      <c r="H84" s="9" t="s">
+      <c r="I84" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="I84" s="9" t="s">
+      <c r="J84" s="9" t="s">
         <v>310</v>
       </c>
-      <c r="J84" s="9" t="s">
-        <v>40</v>
-      </c>
       <c r="K84" s="9" t="s">
         <v>40</v>
       </c>
-      <c r="L84" s="47"/>
-    </row>
-    <row r="85" spans="1:12">
-      <c r="A85" s="45"/>
-      <c r="B85" s="45"/>
-      <c r="C85" s="45"/>
-      <c r="D85" s="45"/>
+      <c r="L84" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="M84" s="48"/>
+    </row>
+    <row r="85" spans="1:13">
+      <c r="A85" s="49"/>
+      <c r="B85" s="49"/>
+      <c r="C85" s="49"/>
+      <c r="D85" s="49"/>
       <c r="E85" s="45"/>
-      <c r="F85" s="9" t="s">
+      <c r="F85" s="49"/>
+      <c r="G85" s="9" t="s">
         <v>274</v>
       </c>
-      <c r="G85" s="9" t="s">
+      <c r="H85" s="9" t="s">
         <v>292</v>
       </c>
-      <c r="H85" s="9" t="s">
+      <c r="I85" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="I85" s="9" t="s">
+      <c r="J85" s="9" t="s">
         <v>311</v>
       </c>
-      <c r="J85" s="9" t="s">
-        <v>40</v>
-      </c>
       <c r="K85" s="9" t="s">
         <v>40</v>
       </c>
-      <c r="L85" s="47"/>
-    </row>
-    <row r="86" spans="1:12">
-      <c r="A86" s="45"/>
-      <c r="B86" s="45"/>
-      <c r="C86" s="45"/>
-      <c r="D86" s="45"/>
+      <c r="L85" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="M85" s="48"/>
+    </row>
+    <row r="86" spans="1:13">
+      <c r="A86" s="49"/>
+      <c r="B86" s="49"/>
+      <c r="C86" s="49"/>
+      <c r="D86" s="49"/>
       <c r="E86" s="45"/>
-      <c r="F86" s="9" t="s">
+      <c r="F86" s="49"/>
+      <c r="G86" s="9" t="s">
         <v>275</v>
       </c>
-      <c r="G86" s="9" t="s">
+      <c r="H86" s="9" t="s">
         <v>293</v>
       </c>
-      <c r="H86" s="9" t="s">
+      <c r="I86" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="I86" s="9" t="s">
+      <c r="J86" s="9" t="s">
         <v>311</v>
       </c>
-      <c r="J86" s="9" t="s">
-        <v>40</v>
-      </c>
       <c r="K86" s="9" t="s">
         <v>40</v>
       </c>
-      <c r="L86" s="47"/>
-    </row>
-    <row r="87" spans="1:12">
-      <c r="A87" s="45"/>
-      <c r="B87" s="45"/>
-      <c r="C87" s="45"/>
-      <c r="D87" s="45"/>
+      <c r="L86" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="M86" s="48"/>
+    </row>
+    <row r="87" spans="1:13">
+      <c r="A87" s="49"/>
+      <c r="B87" s="49"/>
+      <c r="C87" s="49"/>
+      <c r="D87" s="49"/>
       <c r="E87" s="45"/>
-      <c r="F87" s="9" t="s">
+      <c r="F87" s="49"/>
+      <c r="G87" s="9" t="s">
         <v>276</v>
       </c>
-      <c r="G87" s="9" t="s">
+      <c r="H87" s="9" t="s">
         <v>294</v>
       </c>
-      <c r="H87" s="9" t="s">
+      <c r="I87" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="I87" s="9" t="s">
+      <c r="J87" s="9" t="s">
         <v>306</v>
       </c>
-      <c r="J87" s="9" t="s">
-        <v>40</v>
-      </c>
       <c r="K87" s="9" t="s">
         <v>40</v>
       </c>
-      <c r="L87" s="47"/>
-    </row>
-    <row r="88" spans="1:12">
-      <c r="A88" s="45"/>
-      <c r="B88" s="45"/>
-      <c r="C88" s="45"/>
-      <c r="D88" s="45"/>
+      <c r="L87" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="M87" s="48"/>
+    </row>
+    <row r="88" spans="1:13">
+      <c r="A88" s="49"/>
+      <c r="B88" s="49"/>
+      <c r="C88" s="49"/>
+      <c r="D88" s="49"/>
       <c r="E88" s="45"/>
-      <c r="F88" s="9" t="s">
+      <c r="F88" s="49"/>
+      <c r="G88" s="9" t="s">
         <v>277</v>
       </c>
-      <c r="G88" s="9" t="s">
+      <c r="H88" s="9" t="s">
         <v>295</v>
       </c>
-      <c r="H88" s="9" t="s">
+      <c r="I88" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="I88" s="9" t="s">
+      <c r="J88" s="9" t="s">
         <v>312</v>
       </c>
-      <c r="J88" s="9" t="s">
-        <v>40</v>
-      </c>
       <c r="K88" s="9" t="s">
         <v>40</v>
       </c>
-      <c r="L88" s="47"/>
-    </row>
-    <row r="89" spans="1:12">
-      <c r="A89" s="45"/>
-      <c r="B89" s="45"/>
-      <c r="C89" s="45"/>
-      <c r="D89" s="45"/>
+      <c r="L88" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="M88" s="48"/>
+    </row>
+    <row r="89" spans="1:13">
+      <c r="A89" s="49"/>
+      <c r="B89" s="49"/>
+      <c r="C89" s="49"/>
+      <c r="D89" s="49"/>
       <c r="E89" s="45"/>
-      <c r="F89" s="9" t="s">
+      <c r="F89" s="49"/>
+      <c r="G89" s="9" t="s">
         <v>278</v>
       </c>
-      <c r="G89" s="9" t="s">
+      <c r="H89" s="9" t="s">
         <v>296</v>
       </c>
-      <c r="H89" s="9" t="s">
+      <c r="I89" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="I89" s="9" t="s">
+      <c r="J89" s="9" t="s">
         <v>313</v>
       </c>
-      <c r="J89" s="9" t="s">
-        <v>40</v>
-      </c>
       <c r="K89" s="9" t="s">
         <v>40</v>
       </c>
-      <c r="L89" s="47"/>
-    </row>
-    <row r="90" spans="1:12">
-      <c r="A90" s="45"/>
-      <c r="B90" s="45"/>
-      <c r="C90" s="45"/>
-      <c r="D90" s="45"/>
+      <c r="L89" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="M89" s="48"/>
+    </row>
+    <row r="90" spans="1:13">
+      <c r="A90" s="49"/>
+      <c r="B90" s="49"/>
+      <c r="C90" s="49"/>
+      <c r="D90" s="49"/>
       <c r="E90" s="45"/>
-      <c r="F90" s="9" t="s">
+      <c r="F90" s="49"/>
+      <c r="G90" s="9" t="s">
         <v>279</v>
       </c>
-      <c r="G90" s="9" t="s">
+      <c r="H90" s="9" t="s">
         <v>297</v>
       </c>
-      <c r="H90" s="9" t="s">
+      <c r="I90" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="I90" s="9" t="s">
+      <c r="J90" s="9" t="s">
         <v>314</v>
       </c>
-      <c r="J90" s="9" t="s">
-        <v>40</v>
-      </c>
       <c r="K90" s="9" t="s">
         <v>40</v>
       </c>
-      <c r="L90" s="47"/>
-    </row>
-    <row r="91" spans="1:12">
-      <c r="A91" s="45"/>
-      <c r="B91" s="45"/>
-      <c r="C91" s="45"/>
-      <c r="D91" s="45"/>
+      <c r="L90" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="M90" s="48"/>
+    </row>
+    <row r="91" spans="1:13">
+      <c r="A91" s="49"/>
+      <c r="B91" s="49"/>
+      <c r="C91" s="49"/>
+      <c r="D91" s="49"/>
       <c r="E91" s="45"/>
-      <c r="F91" s="9" t="s">
+      <c r="F91" s="49"/>
+      <c r="G91" s="9" t="s">
         <v>280</v>
       </c>
-      <c r="G91" s="9" t="s">
+      <c r="H91" s="9" t="s">
         <v>298</v>
       </c>
-      <c r="H91" s="9" t="s">
+      <c r="I91" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="I91" s="9" t="s">
+      <c r="J91" s="9" t="s">
         <v>309</v>
       </c>
-      <c r="J91" s="9" t="s">
-        <v>40</v>
-      </c>
       <c r="K91" s="9" t="s">
         <v>40</v>
       </c>
-      <c r="L91" s="47"/>
-    </row>
-    <row r="92" spans="1:12">
-      <c r="A92" s="45"/>
-      <c r="B92" s="45"/>
-      <c r="C92" s="45"/>
-      <c r="D92" s="45"/>
+      <c r="L91" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="M91" s="48"/>
+    </row>
+    <row r="92" spans="1:13">
+      <c r="A92" s="49"/>
+      <c r="B92" s="49"/>
+      <c r="C92" s="49"/>
+      <c r="D92" s="49"/>
       <c r="E92" s="45"/>
-      <c r="F92" s="9" t="s">
+      <c r="F92" s="49"/>
+      <c r="G92" s="9" t="s">
         <v>282</v>
       </c>
-      <c r="G92" s="9" t="s">
+      <c r="H92" s="9" t="s">
         <v>299</v>
       </c>
-      <c r="H92" s="9" t="s">
+      <c r="I92" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="I92" s="9" t="s">
+      <c r="J92" s="9" t="s">
         <v>311</v>
       </c>
-      <c r="J92" s="9" t="s">
-        <v>40</v>
-      </c>
       <c r="K92" s="9" t="s">
         <v>40</v>
       </c>
-      <c r="L92" s="47"/>
-    </row>
-    <row r="93" spans="1:12">
-      <c r="A93" s="45"/>
-      <c r="B93" s="45"/>
-      <c r="C93" s="45"/>
-      <c r="D93" s="45"/>
+      <c r="L92" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="M92" s="48"/>
+    </row>
+    <row r="93" spans="1:13">
+      <c r="A93" s="49"/>
+      <c r="B93" s="49"/>
+      <c r="C93" s="49"/>
+      <c r="D93" s="49"/>
       <c r="E93" s="45"/>
-      <c r="F93" s="9" t="s">
+      <c r="F93" s="49"/>
+      <c r="G93" s="9" t="s">
         <v>281</v>
       </c>
-      <c r="G93" s="9" t="s">
+      <c r="H93" s="9" t="s">
         <v>299</v>
       </c>
-      <c r="H93" s="9" t="s">
+      <c r="I93" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="I93" s="9" t="s">
+      <c r="J93" s="9" t="s">
         <v>306</v>
       </c>
-      <c r="J93" s="9" t="s">
-        <v>40</v>
-      </c>
       <c r="K93" s="9" t="s">
         <v>40</v>
       </c>
-      <c r="L93" s="47"/>
-    </row>
-    <row r="94" spans="1:12">
-      <c r="A94" s="45"/>
-      <c r="B94" s="45"/>
-      <c r="C94" s="45"/>
-      <c r="D94" s="45"/>
+      <c r="L93" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="M93" s="48"/>
+    </row>
+    <row r="94" spans="1:13">
+      <c r="A94" s="49"/>
+      <c r="B94" s="49"/>
+      <c r="C94" s="49"/>
+      <c r="D94" s="49"/>
       <c r="E94" s="45"/>
-      <c r="F94" s="9" t="s">
+      <c r="F94" s="49"/>
+      <c r="G94" s="9" t="s">
         <v>283</v>
       </c>
-      <c r="G94" s="9" t="s">
+      <c r="H94" s="9" t="s">
         <v>299</v>
       </c>
-      <c r="H94" s="9" t="s">
+      <c r="I94" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="I94" s="9" t="s">
+      <c r="J94" s="9" t="s">
         <v>315</v>
       </c>
-      <c r="J94" s="9" t="s">
-        <v>40</v>
-      </c>
       <c r="K94" s="9" t="s">
         <v>40</v>
       </c>
-      <c r="L94" s="47"/>
-    </row>
-    <row r="95" spans="1:12">
-      <c r="A95" s="45"/>
-      <c r="B95" s="45" t="s">
+      <c r="L94" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="M94" s="48"/>
+    </row>
+    <row r="95" spans="1:13">
+      <c r="A95" s="49"/>
+      <c r="B95" s="49" t="s">
         <v>406</v>
       </c>
-      <c r="C95" s="45" t="s">
+      <c r="C95" s="49" t="s">
         <v>407</v>
       </c>
-      <c r="D95" s="48" t="s">
+      <c r="D95" s="50" t="s">
+        <v>431</v>
+      </c>
+      <c r="E95" s="46" t="s">
+        <v>428</v>
+      </c>
+      <c r="F95" s="49" t="s">
+        <v>408</v>
+      </c>
+      <c r="G95" s="9" t="s">
+        <v>213</v>
+      </c>
+      <c r="H95" s="9" t="s">
+        <v>179</v>
+      </c>
+      <c r="I95" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="J95" s="9" t="s">
+        <v>217</v>
+      </c>
+      <c r="K95" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="L95" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="M95" s="47" t="s">
         <v>425</v>
       </c>
-      <c r="E95" s="45" t="s">
-        <v>408</v>
-      </c>
-      <c r="F95" s="9" t="s">
-        <v>213</v>
-      </c>
-      <c r="G95" s="9" t="s">
-        <v>179</v>
-      </c>
-      <c r="H95" s="9" t="s">
-        <v>6</v>
-      </c>
-      <c r="I95" s="9" t="s">
-        <v>217</v>
-      </c>
-      <c r="J95" s="9" t="s">
-        <v>40</v>
-      </c>
-      <c r="K95" s="9" t="s">
-        <v>40</v>
-      </c>
-      <c r="L95" s="46" t="s">
-        <v>426</v>
-      </c>
-    </row>
-    <row r="96" spans="1:12">
-      <c r="A96" s="45"/>
-      <c r="B96" s="45"/>
-      <c r="C96" s="45"/>
-      <c r="D96" s="45"/>
-      <c r="E96" s="45"/>
-      <c r="F96" s="9" t="s">
+    </row>
+    <row r="96" spans="1:13" ht="28.5">
+      <c r="A96" s="49"/>
+      <c r="B96" s="49"/>
+      <c r="C96" s="49"/>
+      <c r="D96" s="49"/>
+      <c r="E96" s="46" t="s">
+        <v>429</v>
+      </c>
+      <c r="F96" s="49"/>
+      <c r="G96" s="9" t="s">
         <v>409</v>
       </c>
-      <c r="G96" s="9" t="s">
+      <c r="H96" s="9" t="s">
         <v>410</v>
       </c>
-      <c r="H96" s="9" t="s">
+      <c r="I96" s="9" t="s">
         <v>411</v>
       </c>
-      <c r="I96" s="9" t="s">
+      <c r="J96" s="9" t="s">
         <v>412</v>
       </c>
-      <c r="J96" s="9" t="s">
-        <v>40</v>
-      </c>
       <c r="K96" s="9" t="s">
         <v>40</v>
       </c>
-      <c r="L96" s="47"/>
-    </row>
-    <row r="97" spans="1:13">
-      <c r="A97" s="45"/>
-      <c r="B97" s="45"/>
-      <c r="C97" s="45"/>
-      <c r="D97" s="45"/>
-      <c r="E97" s="45"/>
-      <c r="F97" s="9" t="s">
+      <c r="L96" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="M96" s="48"/>
+    </row>
+    <row r="97" spans="1:14">
+      <c r="A97" s="49"/>
+      <c r="B97" s="49"/>
+      <c r="C97" s="49"/>
+      <c r="D97" s="49"/>
+      <c r="E97" s="45" t="s">
+        <v>430</v>
+      </c>
+      <c r="F97" s="49"/>
+      <c r="G97" s="9" t="s">
         <v>413</v>
       </c>
-      <c r="G97" s="9" t="s">
+      <c r="H97" s="9" t="s">
         <v>414</v>
       </c>
-      <c r="H97" s="9" t="s">
+      <c r="I97" s="9" t="s">
         <v>411</v>
       </c>
-      <c r="I97" s="9" t="s">
+      <c r="J97" s="9" t="s">
         <v>199</v>
       </c>
-      <c r="J97" s="9" t="s">
-        <v>40</v>
-      </c>
       <c r="K97" s="9" t="s">
         <v>40</v>
       </c>
-      <c r="L97" s="47"/>
-    </row>
-    <row r="98" spans="1:13" ht="77.25" customHeight="1">
-      <c r="A98" s="45"/>
-      <c r="B98" s="45"/>
-      <c r="C98" s="45"/>
-      <c r="D98" s="45"/>
-      <c r="E98" s="45"/>
-      <c r="F98" s="9" t="s">
+      <c r="L97" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="M97" s="48"/>
+    </row>
+    <row r="98" spans="1:14" ht="77.25" customHeight="1">
+      <c r="A98" s="49"/>
+      <c r="B98" s="49"/>
+      <c r="C98" s="49"/>
+      <c r="D98" s="49"/>
+      <c r="E98" s="46" t="s">
+        <v>432</v>
+      </c>
+      <c r="F98" s="49"/>
+      <c r="G98" s="9" t="s">
         <v>415</v>
       </c>
-      <c r="G98" s="9" t="s">
+      <c r="H98" s="9" t="s">
         <v>416</v>
       </c>
-      <c r="H98" s="9" t="s">
+      <c r="I98" s="9" t="s">
         <v>411</v>
       </c>
-      <c r="I98" s="9" t="s">
+      <c r="J98" s="9" t="s">
         <v>418</v>
       </c>
-      <c r="J98" s="9" t="s">
-        <v>40</v>
-      </c>
       <c r="K98" s="9" t="s">
         <v>40</v>
       </c>
-      <c r="L98" s="47"/>
-      <c r="M98" s="43" t="s">
+      <c r="L98" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="M98" s="48"/>
+      <c r="N98" s="43" t="s">
         <v>417</v>
       </c>
     </row>
-    <row r="99" spans="1:13" ht="18.75" customHeight="1">
-      <c r="A99" s="45"/>
-      <c r="B99" s="45"/>
-      <c r="C99" s="45"/>
-      <c r="D99" s="45"/>
+    <row r="99" spans="1:14" ht="18.75" customHeight="1">
+      <c r="A99" s="49"/>
+      <c r="B99" s="49"/>
+      <c r="C99" s="49"/>
+      <c r="D99" s="49"/>
       <c r="E99" s="45"/>
-      <c r="F99" s="9" t="s">
+      <c r="F99" s="49"/>
+      <c r="G99" s="9" t="s">
         <v>419</v>
       </c>
-      <c r="G99" s="9" t="s">
+      <c r="H99" s="9" t="s">
         <v>420</v>
       </c>
-      <c r="H99" s="9" t="s">
+      <c r="I99" s="9" t="s">
         <v>411</v>
       </c>
-      <c r="I99" s="9" t="s">
+      <c r="J99" s="9" t="s">
         <v>421</v>
       </c>
-      <c r="J99" s="9" t="s">
-        <v>40</v>
-      </c>
       <c r="K99" s="9" t="s">
         <v>40</v>
       </c>
-      <c r="L99" s="47"/>
-    </row>
-    <row r="100" spans="1:13" ht="17.25" customHeight="1">
-      <c r="A100" s="45"/>
-      <c r="B100" s="45"/>
-      <c r="C100" s="45"/>
-      <c r="D100" s="45"/>
+      <c r="L99" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="M99" s="48"/>
+    </row>
+    <row r="100" spans="1:14" ht="17.25" customHeight="1">
+      <c r="A100" s="49"/>
+      <c r="B100" s="49"/>
+      <c r="C100" s="49"/>
+      <c r="D100" s="49"/>
       <c r="E100" s="45"/>
-      <c r="F100" s="9" t="s">
+      <c r="F100" s="49"/>
+      <c r="G100" s="9" t="s">
         <v>422</v>
       </c>
-      <c r="G100" s="9" t="s">
+      <c r="H100" s="9" t="s">
         <v>423</v>
       </c>
-      <c r="H100" s="9" t="s">
+      <c r="I100" s="9" t="s">
         <v>411</v>
       </c>
-      <c r="I100" s="9" t="s">
+      <c r="J100" s="9" t="s">
         <v>424</v>
       </c>
-      <c r="J100" s="9" t="s">
-        <v>40</v>
-      </c>
       <c r="K100" s="9" t="s">
         <v>40</v>
       </c>
-      <c r="L100" s="47"/>
-    </row>
-    <row r="101" spans="1:13" s="33" customFormat="1">
-      <c r="A101" s="45"/>
+      <c r="L100" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="M100" s="48"/>
+    </row>
+    <row r="101" spans="1:14" s="33" customFormat="1">
+      <c r="A101" s="49"/>
       <c r="B101" s="30" t="s">
         <v>105</v>
       </c>
@@ -5464,60 +5598,41 @@
       <c r="D101" s="30" t="s">
         <v>142</v>
       </c>
-      <c r="E101" s="31"/>
-      <c r="F101" s="32"/>
+      <c r="E101" s="30"/>
+      <c r="F101" s="31"/>
       <c r="G101" s="32"/>
       <c r="H101" s="32"/>
       <c r="I101" s="32"/>
       <c r="J101" s="32"/>
       <c r="K101" s="32"/>
-      <c r="L101" s="31" t="s">
+      <c r="L101" s="32"/>
+      <c r="M101" s="31" t="s">
         <v>140</v>
       </c>
-      <c r="M101" s="32"/>
-    </row>
-    <row r="107" spans="1:13">
-      <c r="K107" s="9" t="s">
+      <c r="N101" s="32"/>
+    </row>
+    <row r="107" spans="1:14">
+      <c r="L107" s="9" t="s">
         <v>212</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="62">
-    <mergeCell ref="L95:L100"/>
-    <mergeCell ref="B58:B62"/>
-    <mergeCell ref="D58:D62"/>
-    <mergeCell ref="E59:E62"/>
-    <mergeCell ref="D53:D57"/>
-    <mergeCell ref="C53:C57"/>
-    <mergeCell ref="B43:B57"/>
-    <mergeCell ref="E54:E57"/>
-    <mergeCell ref="B95:B100"/>
-    <mergeCell ref="C95:C100"/>
-    <mergeCell ref="D95:D100"/>
-    <mergeCell ref="E95:E100"/>
-    <mergeCell ref="B63:B94"/>
-    <mergeCell ref="D63:D94"/>
-    <mergeCell ref="L2:L5"/>
-    <mergeCell ref="L6:L7"/>
-    <mergeCell ref="L9:L12"/>
-    <mergeCell ref="L13:L21"/>
-    <mergeCell ref="L22:L29"/>
-    <mergeCell ref="A63:A101"/>
-    <mergeCell ref="A22:A37"/>
-    <mergeCell ref="E20:E21"/>
-    <mergeCell ref="D13:D21"/>
-    <mergeCell ref="C13:C21"/>
-    <mergeCell ref="B13:B21"/>
-    <mergeCell ref="E22:E29"/>
-    <mergeCell ref="D22:D29"/>
-    <mergeCell ref="C22:C29"/>
-    <mergeCell ref="B22:B29"/>
-    <mergeCell ref="A40:A62"/>
-    <mergeCell ref="A9:A21"/>
-    <mergeCell ref="E32:E34"/>
-    <mergeCell ref="D30:D34"/>
-    <mergeCell ref="B30:B34"/>
-    <mergeCell ref="C63:C94"/>
+    <mergeCell ref="M53:M57"/>
+    <mergeCell ref="C58:C62"/>
+    <mergeCell ref="N38:N39"/>
+    <mergeCell ref="M38:M39"/>
+    <mergeCell ref="C43:C52"/>
+    <mergeCell ref="D43:D52"/>
+    <mergeCell ref="F43:F52"/>
+    <mergeCell ref="M43:M51"/>
+    <mergeCell ref="M58:M62"/>
+    <mergeCell ref="B38:B39"/>
+    <mergeCell ref="C30:C39"/>
+    <mergeCell ref="D38:D39"/>
+    <mergeCell ref="M30:M34"/>
+    <mergeCell ref="F9:F12"/>
+    <mergeCell ref="F16:F19"/>
     <mergeCell ref="B6:B7"/>
     <mergeCell ref="C6:C7"/>
     <mergeCell ref="D6:D7"/>
@@ -5528,23 +5643,43 @@
     <mergeCell ref="D2:D5"/>
     <mergeCell ref="B2:B5"/>
     <mergeCell ref="C2:C5"/>
-    <mergeCell ref="B38:B39"/>
-    <mergeCell ref="C30:C39"/>
-    <mergeCell ref="D38:D39"/>
-    <mergeCell ref="L30:L34"/>
-    <mergeCell ref="E9:E12"/>
-    <mergeCell ref="E16:E19"/>
-    <mergeCell ref="E63:E94"/>
-    <mergeCell ref="L63:L94"/>
-    <mergeCell ref="L53:L57"/>
-    <mergeCell ref="C58:C62"/>
-    <mergeCell ref="M38:M39"/>
-    <mergeCell ref="L38:L39"/>
-    <mergeCell ref="C43:C52"/>
-    <mergeCell ref="D43:D52"/>
-    <mergeCell ref="E43:E52"/>
-    <mergeCell ref="L43:L51"/>
-    <mergeCell ref="L58:L62"/>
+    <mergeCell ref="A63:A101"/>
+    <mergeCell ref="A22:A37"/>
+    <mergeCell ref="F20:F21"/>
+    <mergeCell ref="D13:D21"/>
+    <mergeCell ref="C13:C21"/>
+    <mergeCell ref="B13:B21"/>
+    <mergeCell ref="F22:F29"/>
+    <mergeCell ref="D22:D29"/>
+    <mergeCell ref="C22:C29"/>
+    <mergeCell ref="B22:B29"/>
+    <mergeCell ref="A40:A62"/>
+    <mergeCell ref="A9:A21"/>
+    <mergeCell ref="F32:F34"/>
+    <mergeCell ref="D30:D34"/>
+    <mergeCell ref="B30:B34"/>
+    <mergeCell ref="C63:C94"/>
+    <mergeCell ref="M2:M5"/>
+    <mergeCell ref="M6:M7"/>
+    <mergeCell ref="M9:M12"/>
+    <mergeCell ref="M13:M21"/>
+    <mergeCell ref="M22:M29"/>
+    <mergeCell ref="M95:M100"/>
+    <mergeCell ref="B58:B62"/>
+    <mergeCell ref="D58:D62"/>
+    <mergeCell ref="F59:F62"/>
+    <mergeCell ref="D53:D57"/>
+    <mergeCell ref="C53:C57"/>
+    <mergeCell ref="B43:B57"/>
+    <mergeCell ref="F54:F57"/>
+    <mergeCell ref="B95:B100"/>
+    <mergeCell ref="C95:C100"/>
+    <mergeCell ref="D95:D100"/>
+    <mergeCell ref="F95:F100"/>
+    <mergeCell ref="B63:B94"/>
+    <mergeCell ref="D63:D94"/>
+    <mergeCell ref="F63:F94"/>
+    <mergeCell ref="M63:M94"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>